<commit_message>
Phase 1 - Part 2: ALU modification is completed and ready to be tested
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1F9E38-7250-4012-9C9D-222D6A8FC24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F2FB48-07B1-417D-8A18-123DDCF813A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="343">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -1016,19 +1016,82 @@
     <t xml:space="preserve">MemtoReg </t>
   </si>
   <si>
-    <t>3'b010</t>
-  </si>
-  <si>
-    <t>3'b110</t>
-  </si>
-  <si>
-    <t>3'b000</t>
-  </si>
-  <si>
-    <t>3'b001</t>
-  </si>
-  <si>
-    <t>3'b111</t>
+    <t>add</t>
+  </si>
+  <si>
+    <t>subtruct</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>set less than</t>
+  </si>
+  <si>
+    <t>4'b1000</t>
+  </si>
+  <si>
+    <t>4'b1001</t>
+  </si>
+  <si>
+    <t>4'b0000</t>
+  </si>
+  <si>
+    <t>4'b0001</t>
+  </si>
+  <si>
+    <t>4'b0010</t>
+  </si>
+  <si>
+    <t>4'b0011</t>
+  </si>
+  <si>
+    <t>4'b0100</t>
+  </si>
+  <si>
+    <t>4'b0110</t>
+  </si>
+  <si>
+    <t>4'b0101</t>
+  </si>
+  <si>
+    <t>4'b0111</t>
+  </si>
+  <si>
+    <t>4'b1010</t>
+  </si>
+  <si>
+    <t>4'b1011</t>
+  </si>
+  <si>
+    <t>4'b1100</t>
+  </si>
+  <si>
+    <t>4'b1101</t>
+  </si>
+  <si>
+    <t>4'b1110</t>
+  </si>
+  <si>
+    <t>4'b1111</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1113,6 +1176,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE7EAED"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -1197,7 +1266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1250,59 +1319,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="35">
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1441,6 +1477,54 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1458,13 +1542,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>595146</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>103430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>1313375</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>85923</xdr:rowOff>
@@ -1502,13 +1586,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>204487</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>67004</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>255068</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>133209</xdr:rowOff>
@@ -1597,62 +1681,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="MemtoReg " dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="Branch" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:N31" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="A1:N31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="I"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="31"/>
+    <tableColumn id="14" xr3:uid="{12C25AB1-0066-4E00-9278-43C546BB7A00}" name="Type" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="MemtoReg " dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="Branch" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:F29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:F29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:F29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:D10" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:C11" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1921,23 +2012,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="2" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" customWidth="1"/>
+    <col min="6" max="6" width="36.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1945,41 +2036,44 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="N1" s="18"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" s="18"/>
+    </row>
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1987,22 +2081,22 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2010,17 +2104,20 @@
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
         <v>310</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
@@ -2028,16 +2125,19 @@
         <v>91</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2045,16 +2145,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2068,17 +2168,20 @@
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
         <v>311</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2086,16 +2189,19 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2103,16 +2209,16 @@
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -2126,17 +2232,20 @@
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
         <v>312</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>0</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2144,16 +2253,19 @@
         <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -2161,16 +2273,19 @@
         <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -2178,16 +2293,19 @@
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2195,40 +2313,43 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>1</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
         <v>311</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>36</v>
       </c>
@@ -2236,16 +2357,19 @@
         <v>37</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -2253,16 +2377,19 @@
         <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -2270,16 +2397,19 @@
         <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2287,16 +2417,19 @@
         <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -2304,16 +2437,19 @@
         <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2321,16 +2457,19 @@
         <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -2338,16 +2477,19 @@
         <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>94</v>
       </c>
@@ -2355,16 +2497,19 @@
         <v>95</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -2372,16 +2517,19 @@
         <v>64</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
@@ -2389,16 +2537,19 @@
         <v>99</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -2406,16 +2557,19 @@
         <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
@@ -2423,16 +2577,19 @@
         <v>71</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -2440,16 +2597,19 @@
         <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
@@ -2457,40 +2617,43 @@
         <v>79</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>1</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>0</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>1</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>0</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>1</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>311</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -2498,16 +2661,19 @@
         <v>83</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
@@ -2515,16 +2681,19 @@
         <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
@@ -2532,16 +2701,19 @@
         <v>103</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -2549,16 +2721,19 @@
         <v>107</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -2566,70 +2741,79 @@
         <v>111</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29">
         <v>1</v>
       </c>
       <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
         <v>0</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>311</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2645,10 +2829,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2695,7 +2879,9 @@
       <c r="E2" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="19" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2713,7 +2899,9 @@
       <c r="E3" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="20" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -2731,7 +2919,9 @@
       <c r="E4" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="19" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2749,7 +2939,9 @@
       <c r="E5" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -2767,7 +2959,9 @@
       <c r="E6" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2785,7 +2979,9 @@
       <c r="E7" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -3019,8 +3215,8 @@
       <c r="E20" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>317</v>
+      <c r="F20" s="19" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3057,8 +3253,8 @@
       <c r="E22" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>318</v>
+      <c r="F22" s="20" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3095,8 +3291,8 @@
       <c r="E24" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>319</v>
+      <c r="F24" s="19" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3115,8 +3311,8 @@
       <c r="E25" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>320</v>
+      <c r="F25" s="20" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -3135,7 +3331,9 @@
       <c r="E26" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -3153,7 +3351,9 @@
       <c r="E27" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -3171,8 +3371,8 @@
       <c r="E28" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>321</v>
+      <c r="F28" s="19" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -3193,7 +3393,130 @@
       </c>
       <c r="F29" s="1"/>
     </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="20"/>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E37" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E38" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E39" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>199</v>
+      </c>
+      <c r="F40" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>203</v>
+      </c>
+      <c r="F41" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E43" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E44" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E45" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E46" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E47" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E48" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E49" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F49" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E50" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F50" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F51" s="20" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F52" s="19" t="s">
+        <v>336</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Revert "Merge branch 'master' into Phase1_Part2_Verify"
This reverts commit dadc0066bf52bb479fb541f8b91196a79bb7a899, reversing
changes made to 7226b1e4e4ff7cf9295b2165b46a7cbdb528dab1.
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F2FB48-07B1-417D-8A18-123DDCF813A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1F9E38-7250-4012-9C9D-222D6A8FC24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="322">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -1016,82 +1016,19 @@
     <t xml:space="preserve">MemtoReg </t>
   </si>
   <si>
-    <t>add</t>
-  </si>
-  <si>
-    <t>subtruct</t>
-  </si>
-  <si>
-    <t>or</t>
-  </si>
-  <si>
-    <t>set less than</t>
-  </si>
-  <si>
-    <t>4'b1000</t>
-  </si>
-  <si>
-    <t>4'b1001</t>
-  </si>
-  <si>
-    <t>4'b0000</t>
-  </si>
-  <si>
-    <t>4'b0001</t>
-  </si>
-  <si>
-    <t>4'b0010</t>
-  </si>
-  <si>
-    <t>4'b0011</t>
-  </si>
-  <si>
-    <t>4'b0100</t>
-  </si>
-  <si>
-    <t>4'b0110</t>
-  </si>
-  <si>
-    <t>4'b0101</t>
-  </si>
-  <si>
-    <t>4'b0111</t>
-  </si>
-  <si>
-    <t>4'b1010</t>
-  </si>
-  <si>
-    <t>4'b1011</t>
-  </si>
-  <si>
-    <t>4'b1100</t>
-  </si>
-  <si>
-    <t>4'b1101</t>
-  </si>
-  <si>
-    <t>4'b1110</t>
-  </si>
-  <si>
-    <t>4'b1111</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>3'b010</t>
+  </si>
+  <si>
+    <t>3'b110</t>
+  </si>
+  <si>
+    <t>3'b000</t>
+  </si>
+  <si>
+    <t>3'b001</t>
+  </si>
+  <si>
+    <t>3'b111</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1090,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1176,12 +1113,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE7EAED"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -1266,7 +1197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1319,26 +1250,59 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="34">
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1477,54 +1441,6 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1542,13 +1458,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>595146</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>103430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1313375</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>85923</xdr:rowOff>
@@ -1586,13 +1502,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>204487</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>67004</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>255068</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>133209</xdr:rowOff>
@@ -1681,69 +1597,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:N31" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A1:N31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="I"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="31"/>
-    <tableColumn id="14" xr3:uid="{12C25AB1-0066-4E00-9278-43C546BB7A00}" name="Type" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="MemtoReg " dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="Branch" dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:M31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="MemtoReg " dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="Branch" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:F29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:F29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:F29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:D10" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:C11" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2012,23 +1921,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" customWidth="1"/>
-    <col min="6" max="6" width="36.5546875" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="36.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2036,44 +1945,41 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>337</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="O1" s="18"/>
-    </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="18"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2081,22 +1987,22 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>338</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
         <v>313</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2104,20 +2010,17 @@
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="s">
+        <v>310</v>
+      </c>
+      <c r="L2">
         <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>310</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
@@ -2125,19 +2028,16 @@
         <v>91</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>340</v>
+        <v>92</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2145,16 +2045,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>341</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
         <v>301</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2168,20 +2068,17 @@
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4">
+      <c r="K4" t="s">
+        <v>311</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>0</v>
       </c>
-      <c r="L4" t="s">
-        <v>311</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2189,19 +2086,16 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>341</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2209,16 +2103,16 @@
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>340</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
         <v>301</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -2232,20 +2126,17 @@
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6">
+      <c r="K6" t="s">
+        <v>312</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="L6" t="s">
-        <v>312</v>
-      </c>
       <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2253,19 +2144,16 @@
         <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>340</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -2273,19 +2161,16 @@
         <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>340</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -2293,19 +2178,16 @@
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>340</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2313,43 +2195,40 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>340</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="1" t="s">
         <v>301</v>
       </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
       <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>1</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10">
+      <c r="K10" t="s">
+        <v>311</v>
+      </c>
+      <c r="L10">
         <v>0</v>
-      </c>
-      <c r="L10" t="s">
-        <v>311</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>36</v>
       </c>
@@ -2357,19 +2236,16 @@
         <v>37</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>340</v>
+        <v>38</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -2377,19 +2253,16 @@
         <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>340</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -2397,19 +2270,16 @@
         <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>340</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2417,19 +2287,16 @@
         <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>340</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -2437,19 +2304,16 @@
         <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>340</v>
+        <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2457,19 +2321,16 @@
         <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>340</v>
+        <v>56</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -2477,19 +2338,16 @@
         <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>340</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>94</v>
       </c>
@@ -2497,19 +2355,16 @@
         <v>95</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="D18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -2517,19 +2372,16 @@
         <v>64</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>339</v>
+        <v>65</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
@@ -2537,19 +2389,16 @@
         <v>99</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>339</v>
+        <v>100</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -2557,19 +2406,16 @@
         <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>338</v>
+        <v>68</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
@@ -2577,19 +2423,16 @@
         <v>71</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>340</v>
+        <v>72</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -2597,19 +2440,16 @@
         <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>340</v>
+        <v>76</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
@@ -2617,43 +2457,40 @@
         <v>79</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>340</v>
+        <v>80</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="1" t="s">
         <v>301</v>
       </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
       <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>1</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>1</v>
       </c>
-      <c r="J24">
+      <c r="K24" t="s">
+        <v>311</v>
+      </c>
+      <c r="L24">
         <v>0</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24" t="s">
-        <v>311</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -2661,19 +2498,16 @@
         <v>83</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>340</v>
+        <v>84</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
@@ -2681,19 +2515,16 @@
         <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>340</v>
+        <v>88</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
@@ -2701,19 +2532,16 @@
         <v>103</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>340</v>
+        <v>104</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F27" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -2721,19 +2549,16 @@
         <v>107</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>340</v>
+        <v>108</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F28" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -2741,79 +2566,70 @@
         <v>111</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>340</v>
+        <v>112</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F29" s="1" t="s">
         <v>301</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <v>1</v>
       </c>
       <c r="J29">
-        <v>1</v>
-      </c>
-      <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29" t="s">
+      <c r="K29" t="s">
         <v>311</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>340</v>
+      <c r="C30" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>340</v>
+      <c r="C31" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2829,10 +2645,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2879,9 +2695,7 @@
       <c r="E2" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>321</v>
-      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2899,9 +2713,7 @@
       <c r="E3" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>322</v>
-      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -2919,9 +2731,7 @@
       <c r="E4" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>331</v>
-      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2939,9 +2749,7 @@
       <c r="E5" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F5" t="s">
-        <v>332</v>
-      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -2959,9 +2767,7 @@
       <c r="E6" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F6" t="s">
-        <v>333</v>
-      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2979,9 +2785,7 @@
       <c r="E7" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F7" t="s">
-        <v>334</v>
-      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -3215,8 +3019,8 @@
       <c r="E20" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F20" s="19" t="s">
-        <v>325</v>
+      <c r="F20" s="1" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3253,8 +3057,8 @@
       <c r="E22" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F22" s="20" t="s">
-        <v>328</v>
+      <c r="F22" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3291,8 +3095,8 @@
       <c r="E24" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F24" s="19" t="s">
-        <v>325</v>
+      <c r="F24" s="1" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3311,8 +3115,8 @@
       <c r="E25" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F25" s="20" t="s">
-        <v>324</v>
+      <c r="F25" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -3331,9 +3135,7 @@
       <c r="E26" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F26" t="s">
-        <v>326</v>
-      </c>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -3351,9 +3153,7 @@
       <c r="E27" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F27" t="s">
-        <v>327</v>
-      </c>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -3371,8 +3171,8 @@
       <c r="E28" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F28" s="19" t="s">
-        <v>330</v>
+      <c r="F28" s="1" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -3393,130 +3193,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F36" s="20"/>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E37" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E38" s="20" t="s">
-        <v>319</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E39" s="19" t="s">
-        <v>317</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E40" t="s">
-        <v>199</v>
-      </c>
-      <c r="F40" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E41" t="s">
-        <v>203</v>
-      </c>
-      <c r="F41" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F42" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E43" s="20" t="s">
-        <v>318</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E44" s="19" t="s">
-        <v>320</v>
-      </c>
-      <c r="F44" s="19" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E45" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E46" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E47" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E48" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="F48" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E49" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="F49" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E50" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="F50" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F51" s="20" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F52" s="19" t="s">
-        <v>336</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Phase 1 Part 2:  NOR, XOR and Shift Opeartions are Designed and Tested
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1F9E38-7250-4012-9C9D-222D6A8FC24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30ED8C77-BE41-4DE7-93A4-C4E5D2FBE9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main ISA" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="330">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -1029,6 +1029,30 @@
   </si>
   <si>
     <t>3'b111</t>
+  </si>
+  <si>
+    <t>4'b0011</t>
+  </si>
+  <si>
+    <t>4'b0100</t>
+  </si>
+  <si>
+    <t>4'b1000</t>
+  </si>
+  <si>
+    <t>4'b1001</t>
+  </si>
+  <si>
+    <t>4'b1010</t>
+  </si>
+  <si>
+    <t>4'b1011</t>
+  </si>
+  <si>
+    <t>4'b1100</t>
+  </si>
+  <si>
+    <t>4'b1101</t>
   </si>
 </sst>
 </file>
@@ -1250,60 +1274,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="34">
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1440,6 +1416,54 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1597,62 +1621,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:M31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="MemtoReg " dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="Branch" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="MemtoReg " dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="Branch" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:F29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:F29" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:F29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:D10" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C11" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1923,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2647,8 +2671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2695,7 +2719,9 @@
       <c r="E2" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2713,7 +2739,9 @@
       <c r="E3" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -2731,7 +2759,9 @@
       <c r="E4" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2749,7 +2779,9 @@
       <c r="E5" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -2767,7 +2799,9 @@
       <c r="E6" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2785,7 +2819,9 @@
       <c r="E7" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -3135,7 +3171,9 @@
       <c r="E26" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -3153,7 +3191,9 @@
       <c r="E27" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">

</xml_diff>

<commit_message>
Phase 1 Part 2: Hi/Lo Register Move Opeartions are designed and Tested
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30ED8C77-BE41-4DE7-93A4-C4E5D2FBE9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0A4EBB-98EA-4674-8627-C7159B2835A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="341">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -1053,6 +1053,39 @@
   </si>
   <si>
     <t>4'b1101</t>
+  </si>
+  <si>
+    <t>[DONE] Phase 1 - Assignement 2</t>
+  </si>
+  <si>
+    <t>lo_hi_select</t>
+  </si>
+  <si>
+    <t>hi_write</t>
+  </si>
+  <si>
+    <t>lo_write</t>
+  </si>
+  <si>
+    <t>hi_select</t>
+  </si>
+  <si>
+    <t>lo_select</t>
+  </si>
+  <si>
+    <t> 2'b01</t>
+  </si>
+  <si>
+    <t> 2'b00</t>
+  </si>
+  <si>
+    <t>2'b11</t>
+  </si>
+  <si>
+    <t>4'b0010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DONE] Phase 1 - Assignement 2 </t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1136,6 +1169,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7EAED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1221,7 +1266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1275,11 +1320,80 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="47">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1391,30 +1505,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1621,62 +1711,81 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:M31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="MemtoReg " dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="Branch" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="MemtoReg " dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="34"/>
+    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="Branch" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:F29" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:F29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:S29" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Phase 1 - Assignement 2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{6E220339-5428-41BB-AD5C-1702965A98CD}" name="lo_hi_select" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{E7BF6538-000F-4221-BEAF-1B1069F544DF}" name="hi_write" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{EB15F963-101B-4FD6-8C35-479C603DBCE6}" name="lo_write" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{B96C025F-6BE7-4A63-8A28-B9122951D973}" name="hi_select" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{585ED190-3E47-430F-B835-ADAC4874BFFD}" name="lo_select" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{A9D2244B-08FE-4D9B-B85E-939B8D1FCDA2}" name="ReWrite" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{0B472683-72C5-483F-A1F5-D2FDA9886CAC}" name="RegDst" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{B2AB814A-4427-483D-92F7-16C5C8659619}" name="AluSrc" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{D97A26D2-BB83-45FD-BF71-881B7F9D981D}" name="MemWrite" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{D1503AC1-DA6F-431E-86E3-3CD8BAD27F47}" name="MemtoReg " dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{03DAA7C4-6940-4324-93F3-3F703363AC9E}" name="AluOp" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{B4769B34-7E40-48A1-81CF-AF31CD8F17DF}" name="Jump" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{804568FB-85BF-40E3-B057-9BD0161489CA}" name="Branch" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:D10" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:C11" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1948,7 +2057,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2669,10 +2778,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2681,9 +2790,14 @@
     <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="5" width="28.44140625" customWidth="1"/>
     <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>122</v>
       </c>
@@ -2702,8 +2816,47 @@
       <c r="F1" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2717,13 +2870,52 @@
         <v>125</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>310</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2737,13 +2929,52 @@
         <v>128</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>310</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2757,13 +2988,52 @@
         <v>131</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>310</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -2777,13 +3047,52 @@
         <v>134</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>310</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -2797,13 +3106,52 @@
         <v>137</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>310</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -2817,13 +3165,52 @@
         <v>212</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>310</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -2840,8 +3227,21 @@
         <v>303</v>
       </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -2858,8 +3258,21 @@
         <v>303</v>
       </c>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>145</v>
       </c>
@@ -2876,8 +3289,21 @@
         <v>299</v>
       </c>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>149</v>
       </c>
@@ -2894,8 +3320,21 @@
         <v>299</v>
       </c>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>152</v>
       </c>
@@ -2909,11 +3348,52 @@
         <v>155</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>311</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>63</v>
       </c>
@@ -2927,11 +3407,52 @@
         <v>158</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>311</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>159</v>
       </c>
@@ -2945,11 +3466,52 @@
         <v>162</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>311</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>163</v>
       </c>
@@ -2963,11 +3525,52 @@
         <v>166</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>311</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>167</v>
       </c>
@@ -2984,8 +3587,21 @@
         <v>303</v>
       </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>171</v>
       </c>
@@ -3002,8 +3618,21 @@
         <v>298</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>174</v>
       </c>
@@ -3020,8 +3649,21 @@
         <v>303</v>
       </c>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>177</v>
       </c>
@@ -3038,8 +3680,21 @@
         <v>298</v>
       </c>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
@@ -3058,8 +3713,47 @@
       <c r="F20" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>310</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
@@ -3076,8 +3770,21 @@
         <v>298</v>
       </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>185</v>
       </c>
@@ -3096,8 +3803,47 @@
       <c r="F22" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>310</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -3114,8 +3860,21 @@
         <v>298</v>
       </c>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -3134,8 +3893,47 @@
       <c r="F24" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>310</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>86</v>
       </c>
@@ -3154,8 +3952,47 @@
       <c r="F25" s="1" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>310</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>197</v>
       </c>
@@ -3169,13 +4006,52 @@
         <v>200</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>310</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>201</v>
       </c>
@@ -3189,13 +4065,52 @@
         <v>204</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>310</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>205</v>
       </c>
@@ -3214,8 +4129,47 @@
       <c r="F28" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>310</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -3232,8 +4186,22 @@
         <v>298</v>
       </c>
       <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Phase 1 Part 2: Mult/Div Instructions are implemented and tested | Jr Instruction is implemented and Tested
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0A4EBB-98EA-4674-8627-C7159B2835A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0724421A-55F9-4DE7-8FBF-53646644AD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="347">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -974,9 +974,6 @@
     <t>Future Implemenentation</t>
   </si>
   <si>
-    <t>Phase 1 - Assignement 2</t>
-  </si>
-  <si>
     <t>RegDst</t>
   </si>
   <si>
@@ -1086,6 +1083,27 @@
   </si>
   <si>
     <t xml:space="preserve">[DONE] Phase 1 - Assignement 2 </t>
+  </si>
+  <si>
+    <t>Phase 1 - Assignement 2 [2]</t>
+  </si>
+  <si>
+    <t>Phase 1 - Assignement 2 [3]</t>
+  </si>
+  <si>
+    <t>Phase 1 - Assignement 2 [4]</t>
+  </si>
+  <si>
+    <t>Phase 1 - Assignement 2 [5]</t>
+  </si>
+  <si>
+    <t>Phase 1 - Assignement 2 [6]</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>PCsrc</t>
   </si>
 </sst>
 </file>
@@ -1332,69 +1350,6 @@
   </cellStyles>
   <dxfs count="47">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1505,6 +1460,69 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1712,7 +1730,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
-  <autoFilter ref="A1:M31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}"/>
+  <autoFilter ref="A1:M31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Phase 1 - Assignement 2 [2]"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="44"/>
     <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="43"/>
@@ -1733,59 +1757,59 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:S29" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:S29" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:S29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}">
     <filterColumn colId="4">
       <filters>
-        <filter val="Phase 1 - Assignement 2"/>
+        <filter val="Phase 1 - Assignement 2 [2]"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{6E220339-5428-41BB-AD5C-1702965A98CD}" name="lo_hi_select" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{E7BF6538-000F-4221-BEAF-1B1069F544DF}" name="hi_write" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{EB15F963-101B-4FD6-8C35-479C603DBCE6}" name="lo_write" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{B96C025F-6BE7-4A63-8A28-B9122951D973}" name="hi_select" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{585ED190-3E47-430F-B835-ADAC4874BFFD}" name="lo_select" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{A9D2244B-08FE-4D9B-B85E-939B8D1FCDA2}" name="ReWrite" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{0B472683-72C5-483F-A1F5-D2FDA9886CAC}" name="RegDst" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{B2AB814A-4427-483D-92F7-16C5C8659619}" name="AluSrc" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{D97A26D2-BB83-45FD-BF71-881B7F9D981D}" name="MemWrite" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{D1503AC1-DA6F-431E-86E3-3CD8BAD27F47}" name="MemtoReg " dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{03DAA7C4-6940-4324-93F3-3F703363AC9E}" name="AluOp" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{B4769B34-7E40-48A1-81CF-AF31CD8F17DF}" name="Jump" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{804568FB-85BF-40E3-B057-9BD0161489CA}" name="Branch" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{6E220339-5428-41BB-AD5C-1702965A98CD}" name="lo_hi_select" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{E7BF6538-000F-4221-BEAF-1B1069F544DF}" name="hi_write" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{EB15F963-101B-4FD6-8C35-479C603DBCE6}" name="lo_write" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{B96C025F-6BE7-4A63-8A28-B9122951D973}" name="hi_select" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{585ED190-3E47-430F-B835-ADAC4874BFFD}" name="lo_select" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{A9D2244B-08FE-4D9B-B85E-939B8D1FCDA2}" name="ReWrite" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{0B472683-72C5-483F-A1F5-D2FDA9886CAC}" name="RegDst" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{B2AB814A-4427-483D-92F7-16C5C8659619}" name="AluSrc" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{D97A26D2-BB83-45FD-BF71-881B7F9D981D}" name="MemWrite" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{D1503AC1-DA6F-431E-86E3-3CD8BAD27F47}" name="MemtoReg " dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{03DAA7C4-6940-4324-93F3-3F703363AC9E}" name="AluOp" dataDxfId="13"/>
+    <tableColumn id="18" xr3:uid="{B4769B34-7E40-48A1-81CF-AF31CD8F17DF}" name="Jump" dataDxfId="12"/>
+    <tableColumn id="19" xr3:uid="{804568FB-85BF-40E3-B057-9BD0161489CA}" name="PCsrc" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:D10" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C11" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2056,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView topLeftCell="B1" zoomScale="127" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2087,32 +2111,32 @@
         <v>300</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="N1" s="18"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2126,7 +2150,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2144,7 +2168,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -2153,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
@@ -2167,10 +2191,10 @@
         <v>93</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2202,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -2225,10 +2249,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2260,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -2269,7 +2293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2283,10 +2307,10 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -2300,10 +2324,10 @@
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -2317,10 +2341,10 @@
         <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2352,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -2361,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>36</v>
       </c>
@@ -2378,7 +2402,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -2392,10 +2416,10 @@
         <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -2412,7 +2436,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2426,10 +2450,10 @@
         <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -2443,10 +2467,10 @@
         <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2460,10 +2484,10 @@
         <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -2477,10 +2501,10 @@
         <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>94</v>
       </c>
@@ -2497,7 +2521,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -2514,7 +2538,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
@@ -2531,7 +2555,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -2545,10 +2569,10 @@
         <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
@@ -2562,10 +2586,10 @@
         <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -2579,10 +2603,10 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
@@ -2614,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2623,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -2640,7 +2664,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
@@ -2657,7 +2681,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
@@ -2671,10 +2695,10 @@
         <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -2688,10 +2712,10 @@
         <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -2723,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -2732,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
@@ -2749,7 +2773,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>118</v>
       </c>
@@ -2781,7 +2805,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2814,46 +2838,46 @@
         <v>300</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="L1" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>331</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>332</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>333</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>335</v>
-      </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="P1" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="M1" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>305</v>
-      </c>
-      <c r="O1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="P1" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q1" s="19" t="s">
+      <c r="R1" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="R1" s="19" t="s">
-        <v>309</v>
-      </c>
       <c r="S1" s="19" t="s">
-        <v>306</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
@@ -2870,13 +2894,13 @@
         <v>125</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -2885,10 +2909,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -2906,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -2929,13 +2953,13 @@
         <v>128</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -2944,10 +2968,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -2965,7 +2989,7 @@
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -2988,13 +3012,13 @@
         <v>131</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -3003,10 +3027,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -3024,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="Q4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -3047,13 +3071,13 @@
         <v>134</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
@@ -3062,10 +3086,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -3083,7 +3107,7 @@
         <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -3106,13 +3130,13 @@
         <v>137</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -3121,10 +3145,10 @@
         <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -3142,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="Q6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -3165,13 +3189,13 @@
         <v>212</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
@@ -3180,10 +3204,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -3201,7 +3225,7 @@
         <v>0</v>
       </c>
       <c r="Q7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -3224,22 +3248,48 @@
         <v>141</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>303</v>
+        <v>329</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -3255,7 +3305,7 @@
         <v>144</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>303</v>
+        <v>340</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -3348,43 +3398,43 @@
         <v>155</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
         <v>310</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="L12" s="1">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1">
-        <v>1</v>
-      </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1">
-        <v>0</v>
-      </c>
-      <c r="P12" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>311</v>
       </c>
       <c r="R12" s="1">
         <v>0</v>
@@ -3407,13 +3457,13 @@
         <v>158</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H13" s="1">
         <v>1</v>
@@ -3422,11 +3472,11 @@
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>337</v>
-      </c>
       <c r="L13" s="1">
         <v>0</v>
       </c>
@@ -3443,7 +3493,7 @@
         <v>0</v>
       </c>
       <c r="Q13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="R13" s="1">
         <v>0</v>
@@ -3466,13 +3516,13 @@
         <v>162</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
@@ -3481,10 +3531,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L14" s="1">
         <v>1</v>
@@ -3502,7 +3552,7 @@
         <v>0</v>
       </c>
       <c r="Q14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="R14" s="1">
         <v>0</v>
@@ -3525,13 +3575,13 @@
         <v>166</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
@@ -3540,10 +3590,10 @@
         <v>1</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L15" s="1">
         <v>0</v>
@@ -3561,7 +3611,7 @@
         <v>0</v>
       </c>
       <c r="Q15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="R15" s="1">
         <v>0</v>
@@ -3570,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>167</v>
       </c>
@@ -3584,22 +3634,50 @@
         <v>170</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
+        <v>339</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -3622,7 +3700,9 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -3632,7 +3712,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>174</v>
       </c>
@@ -3646,22 +3726,50 @@
         <v>213</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
+        <v>339</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -3684,7 +3792,9 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="K19" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -3711,10 +3821,10 @@
         <v>301</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
@@ -3723,10 +3833,10 @@
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -3744,7 +3854,7 @@
         <v>0</v>
       </c>
       <c r="Q20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -3801,10 +3911,10 @@
         <v>301</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -3813,10 +3923,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -3834,7 +3944,7 @@
         <v>0</v>
       </c>
       <c r="Q22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R22">
         <v>0</v>
@@ -3891,10 +4001,10 @@
         <v>301</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
@@ -3903,10 +4013,10 @@
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -3924,7 +4034,7 @@
         <v>0</v>
       </c>
       <c r="Q24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R24">
         <v>0</v>
@@ -3950,10 +4060,10 @@
         <v>301</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H25" s="1">
         <v>0</v>
@@ -3962,10 +4072,10 @@
         <v>0</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L25">
         <v>1</v>
@@ -3983,7 +4093,7 @@
         <v>0</v>
       </c>
       <c r="Q25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -4006,13 +4116,13 @@
         <v>200</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
@@ -4021,10 +4131,10 @@
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L26">
         <v>1</v>
@@ -4042,7 +4152,7 @@
         <v>0</v>
       </c>
       <c r="Q26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R26">
         <v>0</v>
@@ -4065,13 +4175,13 @@
         <v>204</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H27" s="1">
         <v>0</v>
@@ -4080,10 +4190,10 @@
         <v>0</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L27">
         <v>1</v>
@@ -4101,7 +4211,7 @@
         <v>0</v>
       </c>
       <c r="Q27" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R27">
         <v>0</v>
@@ -4127,10 +4237,10 @@
         <v>301</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H28" s="1">
         <v>0</v>
@@ -4139,10 +4249,10 @@
         <v>0</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L28">
         <v>1</v>
@@ -4160,7 +4270,7 @@
         <v>0</v>
       </c>
       <c r="Q28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R28">
         <v>0</v>

</xml_diff>

<commit_message>
Phase 1 Part 1: ALL Jump Operations are Complete and Tested
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0724421A-55F9-4DE7-8FBF-53646644AD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C5DB14-275D-4E0D-92FF-0AE93AD13B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main ISA" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="349">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -980,9 +980,6 @@
     <t>AluSrc</t>
   </si>
   <si>
-    <t>Branch</t>
-  </si>
-  <si>
     <t>MemWrite</t>
   </si>
   <si>
@@ -1010,9 +1007,6 @@
     <t>ReWrite</t>
   </si>
   <si>
-    <t xml:space="preserve">MemtoReg </t>
-  </si>
-  <si>
     <t>3'b010</t>
   </si>
   <si>
@@ -1055,9 +1049,6 @@
     <t>[DONE] Phase 1 - Assignement 2</t>
   </si>
   <si>
-    <t>lo_hi_select</t>
-  </si>
-  <si>
     <t>hi_write</t>
   </si>
   <si>
@@ -1104,6 +1095,21 @@
   </si>
   <si>
     <t>PCsrc</t>
+  </si>
+  <si>
+    <t>3'b100</t>
+  </si>
+  <si>
+    <t>Write_Back_sel</t>
+  </si>
+  <si>
+    <t>Write_back_sel</t>
+  </si>
+  <si>
+    <t>PC Src</t>
+  </si>
+  <si>
+    <t>[DONE] Phase 1 - Assignement 1 [3]</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1154,12 +1160,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1284,7 +1284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1337,7 +1337,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1348,7 +1347,43 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="50">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1490,43 +1525,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1729,87 +1737,85 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
-  <autoFilter ref="A1:M31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:Q31" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+  <autoFilter ref="A1:Q31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}">
     <filterColumn colId="4">
       <filters>
-        <filter val="Phase 1 - Assignement 2 [2]"/>
+        <filter val="[DONE] Phase 1 - Assignement 1 [3]"/>
+        <filter val="Phase 1 - Assignement 2 [3]"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="MemtoReg " dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="34"/>
-    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="33"/>
-    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="Branch" dataDxfId="32"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="Write_back_sel" dataDxfId="38"/>
+    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="37"/>
+    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="36"/>
+    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="PC Src" dataDxfId="35"/>
+    <tableColumn id="14" xr3:uid="{65386F80-7AF9-4CF2-BDE0-29D2094B577A}" name="hi_write" dataDxfId="34"/>
+    <tableColumn id="15" xr3:uid="{FA558C62-1F5B-4CE1-A1DE-149585FE9142}" name="lo_write" dataDxfId="33"/>
+    <tableColumn id="16" xr3:uid="{D1B88377-9E5B-4D25-B01D-35C955F02CF0}" name="hi_select" dataDxfId="32"/>
+    <tableColumn id="17" xr3:uid="{F28DE1E5-F9D3-44FC-AA82-3DBE9E42FAEC}" name="lo_select" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:S29" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:S29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Phase 1 - Assignement 2 [2]"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{6E220339-5428-41BB-AD5C-1702965A98CD}" name="lo_hi_select" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{E7BF6538-000F-4221-BEAF-1B1069F544DF}" name="hi_write" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{EB15F963-101B-4FD6-8C35-479C603DBCE6}" name="lo_write" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{B96C025F-6BE7-4A63-8A28-B9122951D973}" name="hi_select" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{585ED190-3E47-430F-B835-ADAC4874BFFD}" name="lo_select" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{A9D2244B-08FE-4D9B-B85E-939B8D1FCDA2}" name="ReWrite" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{0B472683-72C5-483F-A1F5-D2FDA9886CAC}" name="RegDst" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{B2AB814A-4427-483D-92F7-16C5C8659619}" name="AluSrc" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{D97A26D2-BB83-45FD-BF71-881B7F9D981D}" name="MemWrite" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{D1503AC1-DA6F-431E-86E3-3CD8BAD27F47}" name="MemtoReg " dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{03DAA7C4-6940-4324-93F3-3F703363AC9E}" name="AluOp" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{B4769B34-7E40-48A1-81CF-AF31CD8F17DF}" name="Jump" dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{804568FB-85BF-40E3-B057-9BD0161489CA}" name="PCsrc" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:R29" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A1:R29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{A9D2244B-08FE-4D9B-B85E-939B8D1FCDA2}" name="ReWrite" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{0B472683-72C5-483F-A1F5-D2FDA9886CAC}" name="RegDst" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{B2AB814A-4427-483D-92F7-16C5C8659619}" name="AluSrc" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{D97A26D2-BB83-45FD-BF71-881B7F9D981D}" name="MemWrite" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{D1503AC1-DA6F-431E-86E3-3CD8BAD27F47}" name="Write_Back_sel" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{03DAA7C4-6940-4324-93F3-3F703363AC9E}" name="AluOp" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{B4769B34-7E40-48A1-81CF-AF31CD8F17DF}" name="Jump" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{804568FB-85BF-40E3-B057-9BD0161489CA}" name="PCsrc" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{E7BF6538-000F-4221-BEAF-1B1069F544DF}" name="hi_write" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{EB15F963-101B-4FD6-8C35-479C603DBCE6}" name="lo_write" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{B96C025F-6BE7-4A63-8A28-B9122951D973}" name="hi_select" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{585ED190-3E47-430F-B835-ADAC4874BFFD}" name="lo_select" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:D10" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:C11" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2078,10 +2084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="127" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="127" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2091,10 +2097,10 @@
     <col min="3" max="3" width="38.6640625" customWidth="1"/>
     <col min="4" max="4" width="32.5546875" customWidth="1"/>
     <col min="5" max="5" width="36.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2111,7 +2117,7 @@
         <v>300</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>303</v>
@@ -2120,23 +2126,34 @@
         <v>304</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>308</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="N1" s="18"/>
-    </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2150,34 +2167,14 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>309</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
@@ -2191,10 +2188,14 @@
         <v>93</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2227,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -2234,8 +2235,20 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2249,10 +2262,46 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>308</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>344</v>
+      </c>
+      <c r="K5" t="s">
+        <v>309</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2266,7 +2315,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>301</v>
+        <v>348</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2284,7 +2333,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -2292,8 +2341,20 @@
       <c r="M6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2307,10 +2368,14 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -2324,10 +2389,14 @@
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -2341,10 +2410,14 @@
         <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2376,7 +2449,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -2384,8 +2457,20 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>36</v>
       </c>
@@ -2401,8 +2486,12 @@
       <c r="E11" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -2416,10 +2505,14 @@
         <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -2435,8 +2528,12 @@
       <c r="E13" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2450,10 +2547,14 @@
         <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -2467,10 +2568,14 @@
         <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2484,10 +2589,14 @@
         <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -2501,10 +2610,14 @@
         <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>94</v>
       </c>
@@ -2520,8 +2633,12 @@
       <c r="E18" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -2537,8 +2654,12 @@
       <c r="E19" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="1:17" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
@@ -2554,8 +2675,12 @@
       <c r="E20" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="1:17" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -2569,10 +2694,14 @@
         <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+    </row>
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
@@ -2586,10 +2715,14 @@
         <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -2603,10 +2736,14 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
@@ -2638,7 +2775,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2646,8 +2783,20 @@
       <c r="M24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -2663,8 +2812,12 @@
       <c r="E25" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
@@ -2680,8 +2833,12 @@
       <c r="E26" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
@@ -2695,10 +2852,14 @@
         <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -2712,10 +2873,14 @@
         <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -2747,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -2755,8 +2920,20 @@
       <c r="M29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
@@ -2772,8 +2949,12 @@
       <c r="E30" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+    </row>
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>118</v>
       </c>
@@ -2789,6 +2970,10 @@
       <c r="E31" s="1" t="s">
         <v>302</v>
       </c>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2802,10 +2987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2813,15 +2998,15 @@
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="5" width="28.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.21875" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.77734375" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" customWidth="1"/>
+    <col min="18" max="18" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>122</v>
       </c>
@@ -2837,50 +3022,47 @@
       <c r="E1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="P1" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="Q1" s="19" t="s">
         <v>331</v>
       </c>
-      <c r="I1" s="20" t="s">
-        <v>332</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>333</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>314</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="P1" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>307</v>
-      </c>
-      <c r="R1" s="19" t="s">
-        <v>308</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R1" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2894,52 +3076,49 @@
         <v>125</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
+        <v>327</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K2" t="s">
+        <v>308</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>309</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2953,52 +3132,49 @@
         <v>128</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
+        <v>327</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K3" t="s">
+        <v>308</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>309</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3012,52 +3188,49 @@
         <v>131</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
+        <v>327</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K4" t="s">
+        <v>308</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>309</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -3071,52 +3244,49 @@
         <v>134</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
+        <v>327</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K5" t="s">
+        <v>308</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>309</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -3130,52 +3300,49 @@
         <v>137</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F6" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K6" t="s">
+        <v>308</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>309</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -3189,52 +3356,49 @@
         <v>212</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
+        <v>327</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K7" t="s">
+        <v>308</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>309</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -3248,14 +3412,16 @@
         <v>141</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
+        <v>327</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -3267,31 +3433,26 @@
         <v>0</v>
       </c>
       <c r="L8" s="1">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>309</v>
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
       </c>
       <c r="O8" s="1">
         <v>0</v>
       </c>
-      <c r="P8" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>0</v>
-      </c>
-      <c r="R8" s="1">
-        <v>1</v>
-      </c>
-      <c r="S8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P8" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -3305,24 +3466,47 @@
         <v>144</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+        <v>337</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>145</v>
       </c>
@@ -3351,9 +3535,8 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>149</v>
       </c>
@@ -3382,9 +3565,8 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-    </row>
-    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>152</v>
       </c>
@@ -3398,31 +3580,31 @@
         <v>155</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G12" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="K12" t="s">
         <v>309</v>
       </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="L12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
@@ -3430,20 +3612,17 @@
       <c r="O12" s="1">
         <v>0</v>
       </c>
-      <c r="P12" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>310</v>
-      </c>
-      <c r="R12" s="1">
-        <v>0</v>
-      </c>
-      <c r="S12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>63</v>
       </c>
@@ -3457,52 +3636,49 @@
         <v>158</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>310</v>
+        <v>336</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="K13" t="s">
+        <v>309</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="L13" s="1">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>310</v>
-      </c>
-      <c r="R13" s="1">
-        <v>0</v>
-      </c>
-      <c r="S13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>159</v>
       </c>
@@ -3516,13 +3692,13 @@
         <v>162</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
@@ -3531,16 +3707,16 @@
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
+      </c>
+      <c r="K14" t="s">
+        <v>309</v>
       </c>
       <c r="L14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="1">
         <v>0</v>
@@ -3548,20 +3724,17 @@
       <c r="O14" s="1">
         <v>0</v>
       </c>
-      <c r="P14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>310</v>
-      </c>
-      <c r="R14" s="1">
-        <v>0</v>
-      </c>
-      <c r="S14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P14" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>163</v>
       </c>
@@ -3575,52 +3748,49 @@
         <v>166</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>310</v>
+        <v>336</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K15" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="K15" t="s">
+        <v>309</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="L15" s="1">
-        <v>0</v>
-      </c>
-      <c r="M15" s="1">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1">
-        <v>0</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>310</v>
-      </c>
-      <c r="R15" s="1">
-        <v>0</v>
-      </c>
-      <c r="S15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>167</v>
       </c>
@@ -3634,25 +3804,25 @@
         <v>170</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>310</v>
+        <v>336</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>337</v>
+        <v>309</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>337</v>
+        <v>309</v>
       </c>
       <c r="L16" s="1">
         <v>0</v>
@@ -3661,25 +3831,22 @@
         <v>0</v>
       </c>
       <c r="N16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="1">
-        <v>0</v>
-      </c>
-      <c r="P16" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>334</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="R16" s="1">
-        <v>0</v>
-      </c>
-      <c r="S16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>171</v>
       </c>
@@ -3700,9 +3867,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="1" t="s">
-        <v>309</v>
-      </c>
+      <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -3710,9 +3875,8 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-    </row>
-    <row r="18" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>174</v>
       </c>
@@ -3726,19 +3890,19 @@
         <v>213</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>310</v>
+        <v>336</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>309</v>
@@ -3753,25 +3917,22 @@
         <v>0</v>
       </c>
       <c r="N18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="1">
-        <v>0</v>
-      </c>
-      <c r="P18" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="R18" s="1">
-        <v>0</v>
-      </c>
-      <c r="S18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>177</v>
       </c>
@@ -3792,9 +3953,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1" t="s">
-        <v>309</v>
-      </c>
+      <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -3802,9 +3961,8 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-    </row>
-    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
@@ -3820,50 +3978,47 @@
       <c r="E20" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K20" t="s">
+        <v>308</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>309</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
@@ -3892,9 +4047,8 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-    </row>
-    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>185</v>
       </c>
@@ -3910,50 +4064,47 @@
       <c r="E22" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K22" t="s">
+        <v>308</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>309</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -3982,9 +4133,8 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -4000,50 +4150,47 @@
       <c r="E24" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K24" t="s">
+        <v>308</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <v>1</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>309</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>86</v>
       </c>
@@ -4059,50 +4206,47 @@
       <c r="E25" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
         <v>0</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K25" t="s">
+        <v>308</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25">
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>309</v>
-      </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>197</v>
       </c>
@@ -4116,52 +4260,49 @@
         <v>200</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H26" s="1">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1">
+        <v>327</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K26" t="s">
+        <v>308</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <v>1</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>309</v>
-      </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>201</v>
       </c>
@@ -4175,52 +4316,49 @@
         <v>204</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
+        <v>327</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
         <v>0</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K27" t="s">
+        <v>308</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27">
-        <v>1</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>309</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>205</v>
       </c>
@@ -4236,50 +4374,47 @@
       <c r="E28" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1">
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
         <v>0</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>336</v>
+        <v>309</v>
+      </c>
+      <c r="K28" t="s">
+        <v>308</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28">
-        <v>1</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>309</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-      <c r="S28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -4308,7 +4443,6 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Phase 1 Part 2: Branch instructions are Completed and Tested
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C5DB14-275D-4E0D-92FF-0AE93AD13B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635389AA-C932-4521-B048-A689A07DE411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="355">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -1079,9 +1079,6 @@
     <t>Phase 1 - Assignement 2 [2]</t>
   </si>
   <si>
-    <t>Phase 1 - Assignement 2 [3]</t>
-  </si>
-  <si>
     <t>Phase 1 - Assignement 2 [4]</t>
   </si>
   <si>
@@ -1109,7 +1106,28 @@
     <t>PC Src</t>
   </si>
   <si>
-    <t>[DONE] Phase 1 - Assignement 1 [3]</t>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>! zero</t>
+  </si>
+  <si>
+    <t>if(rt ==0) ltz else gez</t>
+  </si>
+  <si>
+    <t>lez</t>
+  </si>
+  <si>
+    <t>gtz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DONE] Phase 1 - Assignement 1 </t>
+  </si>
+  <si>
+    <t>[DONE] Phase 1 - Assignement 1 [6]</t>
+  </si>
+  <si>
+    <t>[DONE] Phase 1 - Assignement 1 [4]</t>
   </si>
 </sst>
 </file>
@@ -1349,42 +1367,6 @@
   </cellStyles>
   <dxfs count="50">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1502,6 +1484,42 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1741,8 +1759,8 @@
   <autoFilter ref="A1:Q31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}">
     <filterColumn colId="4">
       <filters>
-        <filter val="[DONE] Phase 1 - Assignement 1 [3]"/>
-        <filter val="Phase 1 - Assignement 2 [3]"/>
+        <filter val="[DONE] Phase 1 - Assignement 1 [4]"/>
+        <filter val="Phase 1 - Assignement 2 [4]"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1778,44 +1796,44 @@
     <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="26"/>
     <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="25"/>
     <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{A9D2244B-08FE-4D9B-B85E-939B8D1FCDA2}" name="ReWrite" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{0B472683-72C5-483F-A1F5-D2FDA9886CAC}" name="RegDst" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{B2AB814A-4427-483D-92F7-16C5C8659619}" name="AluSrc" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{D97A26D2-BB83-45FD-BF71-881B7F9D981D}" name="MemWrite" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{D1503AC1-DA6F-431E-86E3-3CD8BAD27F47}" name="Write_Back_sel" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{03DAA7C4-6940-4324-93F3-3F703363AC9E}" name="AluOp" dataDxfId="7"/>
-    <tableColumn id="18" xr3:uid="{B4769B34-7E40-48A1-81CF-AF31CD8F17DF}" name="Jump" dataDxfId="6"/>
-    <tableColumn id="19" xr3:uid="{804568FB-85BF-40E3-B057-9BD0161489CA}" name="PCsrc" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{E7BF6538-000F-4221-BEAF-1B1069F544DF}" name="hi_write" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{EB15F963-101B-4FD6-8C35-479C603DBCE6}" name="lo_write" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{B96C025F-6BE7-4A63-8A28-B9122951D973}" name="hi_select" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{585ED190-3E47-430F-B835-ADAC4874BFFD}" name="lo_select" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{A9D2244B-08FE-4D9B-B85E-939B8D1FCDA2}" name="ReWrite" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{0B472683-72C5-483F-A1F5-D2FDA9886CAC}" name="RegDst" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{B2AB814A-4427-483D-92F7-16C5C8659619}" name="AluSrc" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{D97A26D2-BB83-45FD-BF71-881B7F9D981D}" name="MemWrite" dataDxfId="20"/>
+    <tableColumn id="16" xr3:uid="{D1503AC1-DA6F-431E-86E3-3CD8BAD27F47}" name="Write_Back_sel" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{03DAA7C4-6940-4324-93F3-3F703363AC9E}" name="AluOp" dataDxfId="18"/>
+    <tableColumn id="18" xr3:uid="{B4769B34-7E40-48A1-81CF-AF31CD8F17DF}" name="Jump" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{804568FB-85BF-40E3-B057-9BD0161489CA}" name="PCsrc" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{E7BF6538-000F-4221-BEAF-1B1069F544DF}" name="hi_write" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{EB15F963-101B-4FD6-8C35-479C603DBCE6}" name="lo_write" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{B96C025F-6BE7-4A63-8A28-B9122951D973}" name="hi_select" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{585ED190-3E47-430F-B835-ADAC4874BFFD}" name="lo_select" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{2C2B3870-9B9E-459D-B78A-1F301F881E15}" name="AluControl" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:D10" xr:uid="{D53E060B-7B9B-43C9-B6C3-0ADAD9EBE1D7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{9277D667-9F6C-4B1A-9BD6-8F4F09DC6FCC}" name="Funct " dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{44121D79-0FB6-4BA0-822D-A22356C92E27}" name="Name " dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9FFE180B-8031-4716-9450-AF517E4275A8}" name="Description " dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{700AEF16-A70F-499B-87D2-32234302488E}" name="Operation" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C11" xr:uid="{4ED1B589-2AD4-4E0A-A923-4EE6DF5E917F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{54084E4B-9E28-4AC8-AF1B-3C8B1A6C439F}" name="Test #" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{BD73A61D-1FF1-4476-B2A3-42E28CFEB520}" name="Function" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{89ABFDA6-6F2C-4281-BB66-65F42B941C05}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2086,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="127" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="127" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2098,6 +2116,7 @@
     <col min="4" max="4" width="32.5546875" customWidth="1"/>
     <col min="5" max="5" width="36.5546875" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -2129,7 +2148,7 @@
         <v>305</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>306</v>
@@ -2138,7 +2157,7 @@
         <v>307</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N1" s="19" t="s">
         <v>328</v>
@@ -2174,7 +2193,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
@@ -2188,12 +2207,44 @@
         <v>93</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+        <v>327</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>310</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>349</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -2277,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K5" t="s">
         <v>309</v>
@@ -2301,7 +2352,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2315,7 +2366,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2338,8 +2389,8 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6">
-        <v>1</v>
+      <c r="M6" t="s">
+        <v>347</v>
       </c>
       <c r="N6" s="1">
         <v>0</v>
@@ -2354,7 +2405,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2368,14 +2419,46 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>310</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>348</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -2389,14 +2472,46 @@
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>310</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>350</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -2410,14 +2525,46 @@
         <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>310</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>351</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2431,7 +2578,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>301</v>
+        <v>354</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2491,7 +2638,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -2505,7 +2652,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -2533,7 +2680,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2547,14 +2694,14 @@
         <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -2568,14 +2715,14 @@
         <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2589,14 +2736,14 @@
         <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -2610,7 +2757,7 @@
         <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -2694,7 +2841,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -2715,7 +2862,7 @@
         <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -2736,7 +2883,7 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -2757,7 +2904,7 @@
         <v>81</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>301</v>
+        <v>353</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -2852,7 +2999,7 @@
         <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -2873,7 +3020,7 @@
         <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -2894,7 +3041,7 @@
         <v>113</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>301</v>
+        <v>353</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3035,7 +3182,7 @@
         <v>305</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K1" s="18" t="s">
         <v>306</v>
@@ -3044,7 +3191,7 @@
         <v>307</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N1" s="19" t="s">
         <v>328</v>
@@ -3418,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>308</v>
@@ -3481,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K9" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Phase 1 Part 2: ALU Immediate Instructions and MUL instruction is Designed and Tested
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635389AA-C932-4521-B048-A689A07DE411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C96AFE3-604A-446F-A8DD-2EB5D55D8B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main ISA" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="354">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -1079,15 +1079,6 @@
     <t>Phase 1 - Assignement 2 [2]</t>
   </si>
   <si>
-    <t>Phase 1 - Assignement 2 [4]</t>
-  </si>
-  <si>
-    <t>Phase 1 - Assignement 2 [5]</t>
-  </si>
-  <si>
-    <t>Phase 1 - Assignement 2 [6]</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -1124,10 +1115,16 @@
     <t xml:space="preserve">[DONE] Phase 1 - Assignement 1 </t>
   </si>
   <si>
-    <t>[DONE] Phase 1 - Assignement 1 [6]</t>
-  </si>
-  <si>
-    <t>[DONE] Phase 1 - Assignement 1 [4]</t>
+    <t>se_select</t>
+  </si>
+  <si>
+    <t>AluOp_immediate</t>
+  </si>
+  <si>
+    <t>3'b011</t>
+  </si>
+  <si>
+    <t>3'b101</t>
   </si>
 </sst>
 </file>
@@ -1755,16 +1752,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:Q31" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="A1:Q31" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:S32" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+  <autoFilter ref="A1:S32" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}">
     <filterColumn colId="4">
       <filters>
-        <filter val="[DONE] Phase 1 - Assignement 1 [4]"/>
-        <filter val="Phase 1 - Assignement 2 [4]"/>
+        <filter val="[DONE] Phase 1 - Assignement 2"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="17">
+  <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="47"/>
     <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="46"/>
     <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="45"/>
@@ -1776,6 +1772,8 @@
     <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="39"/>
     <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="Write_back_sel" dataDxfId="38"/>
     <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="37"/>
+    <tableColumn id="20" xr3:uid="{4B7A4639-28F0-4297-B746-1FB610AB5BC3}" name="AluOp_immediate"/>
+    <tableColumn id="21" xr3:uid="{83AF33B5-363D-492B-8E5C-C63E2DB98A90}" name="se_select"/>
     <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="36"/>
     <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="PC Src" dataDxfId="35"/>
     <tableColumn id="14" xr3:uid="{65386F80-7AF9-4CF2-BDE0-29D2094B577A}" name="hi_write" dataDxfId="34"/>
@@ -1789,7 +1787,13 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:R29" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="A1:R29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}"/>
+  <autoFilter ref="A1:R29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="[DONE] Phase 1 - Assignement 2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="27"/>
@@ -2102,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="127" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="127" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2116,10 +2120,10 @@
     <col min="4" max="4" width="32.5546875" customWidth="1"/>
     <col min="5" max="5" width="36.5546875" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2148,31 +2152,37 @@
         <v>305</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>306</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="N1" s="19" t="s">
+      <c r="O1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="P1" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="R1" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2188,12 +2198,12 @@
       <c r="E2" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
@@ -2227,26 +2237,26 @@
       <c r="K3" t="s">
         <v>310</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3" t="s">
-        <v>349</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>346</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2280,26 +2290,26 @@
       <c r="K4" t="s">
         <v>309</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1">
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2328,31 +2338,31 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K5" t="s">
         <v>309</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2366,7 +2376,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2386,26 +2396,26 @@
       <c r="K6" t="s">
         <v>310</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
-        <v>347</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>344</v>
       </c>
       <c r="P6" s="1">
         <v>0</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2439,26 +2449,26 @@
       <c r="K7" t="s">
         <v>310</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s">
-        <v>348</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0</v>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>345</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -2492,26 +2502,26 @@
       <c r="K8" t="s">
         <v>310</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
-        <v>350</v>
-      </c>
-      <c r="N8" s="1">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1">
-        <v>0</v>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>347</v>
       </c>
       <c r="P8" s="1">
         <v>0</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -2545,26 +2555,26 @@
       <c r="K9" t="s">
         <v>310</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
-        <v>351</v>
-      </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1">
-        <v>0</v>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>348</v>
       </c>
       <c r="P9" s="1">
         <v>0</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2578,7 +2588,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>354</v>
+        <v>301</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2596,28 +2606,34 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
+        <v>334</v>
+      </c>
+      <c r="L10" t="s">
+        <v>316</v>
+      </c>
+      <c r="M10" t="s">
         <v>309</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1">
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" s="1">
         <v>0</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>36</v>
       </c>
@@ -2633,12 +2649,12 @@
       <c r="E11" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -2652,14 +2668,52 @@
         <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>334</v>
+      </c>
+      <c r="L12" t="s">
+        <v>317</v>
+      </c>
+      <c r="M12" t="s">
+        <v>309</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -2675,12 +2729,12 @@
       <c r="E13" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2694,14 +2748,52 @@
         <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>334</v>
+      </c>
+      <c r="L14" t="s">
+        <v>314</v>
+      </c>
+      <c r="M14" t="s">
+        <v>310</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -2715,14 +2807,52 @@
         <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>334</v>
+      </c>
+      <c r="L15" t="s">
+        <v>352</v>
+      </c>
+      <c r="M15" t="s">
+        <v>310</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2736,14 +2866,52 @@
         <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>334</v>
+      </c>
+      <c r="L16" t="s">
+        <v>340</v>
+      </c>
+      <c r="M16" t="s">
+        <v>310</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -2757,14 +2925,52 @@
         <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
         <v>338</v>
       </c>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>338</v>
+      </c>
+      <c r="J17" t="s">
+        <v>353</v>
+      </c>
+      <c r="K17" t="s">
+        <v>338</v>
+      </c>
+      <c r="L17" t="s">
+        <v>338</v>
+      </c>
+      <c r="M17" t="s">
+        <v>308</v>
+      </c>
+      <c r="N17" t="s">
+        <v>338</v>
+      </c>
+      <c r="O17" t="s">
+        <v>338</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>94</v>
       </c>
@@ -2780,12 +2986,12 @@
       <c r="E18" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -2801,12 +3007,12 @@
       <c r="E19" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
@@ -2822,12 +3028,12 @@
       <c r="E20" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -2841,14 +3047,52 @@
         <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>338</v>
+      </c>
+      <c r="I21" t="s">
+        <v>338</v>
+      </c>
+      <c r="J21" t="s">
+        <v>315</v>
+      </c>
+      <c r="K21" t="s">
+        <v>338</v>
+      </c>
+      <c r="L21" t="s">
+        <v>338</v>
+      </c>
+      <c r="M21" t="s">
+        <v>338</v>
+      </c>
+      <c r="N21" t="s">
+        <v>338</v>
+      </c>
+      <c r="O21" t="s">
+        <v>338</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
@@ -2862,14 +3106,14 @@
         <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+        <v>298</v>
+      </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -2883,14 +3127,14 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
+        <v>298</v>
+      </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
@@ -2904,7 +3148,7 @@
         <v>81</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -2924,26 +3168,26 @@
       <c r="K24" t="s">
         <v>309</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1">
-        <v>0</v>
-      </c>
-      <c r="O24" s="1">
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
         <v>0</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="Q24" s="1">
+        <v>0</v>
+      </c>
+      <c r="R24" s="1">
+        <v>0</v>
+      </c>
+      <c r="S24" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -2959,12 +3203,12 @@
       <c r="E25" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-    </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
@@ -2980,12 +3224,12 @@
       <c r="E26" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-    </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+    </row>
+    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
@@ -2999,14 +3243,14 @@
         <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
+        <v>298</v>
+      </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-    </row>
-    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+    </row>
+    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -3020,14 +3264,14 @@
         <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
+        <v>298</v>
+      </c>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-    </row>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+    </row>
+    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -3041,7 +3285,7 @@
         <v>113</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3061,26 +3305,26 @@
       <c r="K29" t="s">
         <v>309</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29" s="1">
-        <v>0</v>
-      </c>
-      <c r="O29" s="1">
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
         <v>0</v>
       </c>
       <c r="P29" s="1">
         <v>0</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0</v>
+      </c>
+      <c r="S29" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
@@ -3096,12 +3340,12 @@
       <c r="E30" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-    </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+    </row>
+    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>118</v>
       </c>
@@ -3117,10 +3361,29 @@
       <c r="E31" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+    </row>
+    <row r="32" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3136,8 +3399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3182,7 +3445,7 @@
         <v>305</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K1" s="18" t="s">
         <v>306</v>
@@ -3191,7 +3454,7 @@
         <v>307</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="N1" s="19" t="s">
         <v>328</v>
@@ -3565,7 +3828,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>308</v>
@@ -3599,7 +3862,7 @@
       </c>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -3628,7 +3891,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K9" s="1">
         <v>0</v>
@@ -3653,7 +3916,7 @@
       </c>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>145</v>
       </c>
@@ -3683,7 +3946,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>149</v>
       </c>
@@ -3993,7 +4256,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>171</v>
       </c>
@@ -4079,7 +4342,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>177</v>
       </c>
@@ -4109,7 +4372,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
@@ -4165,7 +4428,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
@@ -4195,7 +4458,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>185</v>
       </c>
@@ -4251,7 +4514,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -4281,7 +4544,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -4337,7 +4600,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>86</v>
       </c>
@@ -4505,7 +4768,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>205</v>
       </c>
@@ -4561,7 +4824,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
Phase 1 Part 3: Assertions for Single Cycle MIPS is Written and Tested except Unsigned and Store Assertions
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C96AFE3-604A-446F-A8DD-2EB5D55D8B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D041EF-96D8-4BC5-856F-53C4762348FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="351">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -959,21 +959,12 @@
 lui, ori</t>
   </si>
   <si>
-    <t>Assignment #3</t>
-  </si>
-  <si>
-    <t>Assignment #5</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
     <t>[DONE] Phase 1 - Assignement 1</t>
   </si>
   <si>
-    <t>Future Implemenentation</t>
-  </si>
-  <si>
     <t>RegDst</t>
   </si>
   <si>
@@ -998,9 +989,6 @@
     <t>2'b01</t>
   </si>
   <si>
-    <t>Phase 1</t>
-  </si>
-  <si>
     <t>AluControl</t>
   </si>
   <si>
@@ -1076,12 +1064,6 @@
     <t xml:space="preserve">[DONE] Phase 1 - Assignement 2 </t>
   </si>
   <si>
-    <t>Phase 1 - Assignement 2 [2]</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>PCsrc</t>
   </si>
   <si>
@@ -1097,9 +1079,6 @@
     <t>PC Src</t>
   </si>
   <si>
-    <t>zero</t>
-  </si>
-  <si>
     <t>! zero</t>
   </si>
   <si>
@@ -1125,6 +1104,18 @@
   </si>
   <si>
     <t>3'b101</t>
+  </si>
+  <si>
+    <t>e_zero</t>
+  </si>
+  <si>
+    <t>Phase 1 - Assignement 3 [1]</t>
+  </si>
+  <si>
+    <t>Phase 1 - Assignement 3 [2]</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1156,13 +1147,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color rgb="FFFFFFFF"/>
       <name val="Aptos"/>
@@ -1171,13 +1155,6 @@
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Aptos"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1299,7 +1276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1316,12 +1293,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1334,23 +1305,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1358,11 +1326,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="49">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1481,9 +1455,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1752,58 +1723,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:S32" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="A1:S32" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="[DONE] Phase 1 - Assignement 2"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:S32" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A1:S32" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="Write_back_sel" dataDxfId="38"/>
-    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{4C0751C6-22DE-48F3-A333-C0824C0F0EFD}" name="Comments" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{599EA1B7-5FC4-4650-9D00-5A65D2D76FD2}" name="ReWrite" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{FADF9286-B678-4102-91DC-1ADDBF050E85}" name="RegDst" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{0CF239B5-36C7-4DBC-8249-487AE1E5F5A5}" name="AluSrc" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{1BC2ABDC-0C79-4111-A3DE-6C63C94FA5D5}" name="MemWrite" dataDxfId="38"/>
+    <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="Write_back_sel" dataDxfId="37"/>
+    <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="36"/>
     <tableColumn id="20" xr3:uid="{4B7A4639-28F0-4297-B746-1FB610AB5BC3}" name="AluOp_immediate"/>
     <tableColumn id="21" xr3:uid="{83AF33B5-363D-492B-8E5C-C63E2DB98A90}" name="se_select"/>
-    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="36"/>
-    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="PC Src" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{65386F80-7AF9-4CF2-BDE0-29D2094B577A}" name="hi_write" dataDxfId="34"/>
-    <tableColumn id="15" xr3:uid="{FA558C62-1F5B-4CE1-A1DE-149585FE9142}" name="lo_write" dataDxfId="33"/>
-    <tableColumn id="16" xr3:uid="{D1B88377-9E5B-4D25-B01D-35C955F02CF0}" name="hi_select" dataDxfId="32"/>
-    <tableColumn id="17" xr3:uid="{F28DE1E5-F9D3-44FC-AA82-3DBE9E42FAEC}" name="lo_select" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="35"/>
+    <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="PC Src" dataDxfId="34"/>
+    <tableColumn id="14" xr3:uid="{65386F80-7AF9-4CF2-BDE0-29D2094B577A}" name="hi_write" dataDxfId="33"/>
+    <tableColumn id="15" xr3:uid="{FA558C62-1F5B-4CE1-A1DE-149585FE9142}" name="lo_write" dataDxfId="32"/>
+    <tableColumn id="16" xr3:uid="{D1B88377-9E5B-4D25-B01D-35C955F02CF0}" name="hi_select" dataDxfId="31"/>
+    <tableColumn id="17" xr3:uid="{F28DE1E5-F9D3-44FC-AA82-3DBE9E42FAEC}" name="lo_select" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:R29" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="A1:R29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="[DONE] Phase 1 - Assignement 2"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{A9D2244B-08FE-4D9B-B85E-939B8D1FCDA2}" name="ReWrite" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{0B472683-72C5-483F-A1F5-D2FDA9886CAC}" name="RegDst" dataDxfId="22"/>
-    <tableColumn id="14" xr3:uid="{B2AB814A-4427-483D-92F7-16C5C8659619}" name="AluSrc" dataDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{D97A26D2-BB83-45FD-BF71-881B7F9D981D}" name="MemWrite" dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:Q29" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A1:Q29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{916118AB-C4A0-47F3-87B2-8F2F5A96272D}" name="Comments" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{A9D2244B-08FE-4D9B-B85E-939B8D1FCDA2}" name="ReWrite" dataDxfId="22"/>
+    <tableColumn id="13" xr3:uid="{0B472683-72C5-483F-A1F5-D2FDA9886CAC}" name="RegDst" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{B2AB814A-4427-483D-92F7-16C5C8659619}" name="AluSrc" dataDxfId="20"/>
     <tableColumn id="16" xr3:uid="{D1503AC1-DA6F-431E-86E3-3CD8BAD27F47}" name="Write_Back_sel" dataDxfId="19"/>
     <tableColumn id="17" xr3:uid="{03DAA7C4-6940-4324-93F3-3F703363AC9E}" name="AluOp" dataDxfId="18"/>
     <tableColumn id="18" xr3:uid="{B4769B34-7E40-48A1-81CF-AF31CD8F17DF}" name="Jump" dataDxfId="17"/>
@@ -2109,7 +2067,7 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView zoomScale="127" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E21"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2120,6 +2078,7 @@
     <col min="4" max="4" width="32.5546875" customWidth="1"/>
     <col min="5" max="5" width="36.5546875" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="12" max="12" width="14.21875" customWidth="1"/>
     <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2137,52 +2096,52 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="P1" s="19" t="s">
-        <v>328</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="R1" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2195,9 +2154,7 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>311</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -2217,7 +2174,7 @@
         <v>93</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2235,28 +2192,20 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>346</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2270,25 +2219,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -2296,18 +2227,10 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>0</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>309</v>
-      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2323,13 +2246,13 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2338,10 +2261,10 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="K5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -2349,20 +2272,12 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>0</v>
-      </c>
-      <c r="R5" s="1">
-        <v>0</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2376,7 +2291,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2387,33 +2302,22 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>344</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1">
-        <v>0</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>309</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2429,7 +2333,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2447,26 +2351,18 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>345</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0</v>
-      </c>
-      <c r="R7" s="1">
-        <v>0</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>309</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -2482,7 +2378,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -2500,26 +2396,18 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>347</v>
-      </c>
-      <c r="P8" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>0</v>
-      </c>
-      <c r="R8" s="1">
-        <v>0</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>309</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -2535,7 +2423,7 @@
         <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2553,28 +2441,20 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>348</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>0</v>
-      </c>
-      <c r="R9" s="1">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2588,7 +2468,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2599,41 +2479,24 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="L10" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="M10" t="s">
-        <v>309</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>0</v>
-      </c>
-      <c r="R10" s="1">
-        <v>0</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>36</v>
       </c>
@@ -2647,7 +2510,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -2668,7 +2531,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -2686,34 +2549,20 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="L12" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="M12" t="s">
-        <v>309</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>0</v>
-      </c>
-      <c r="R12" s="1">
-        <v>0</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -2727,7 +2576,7 @@
         <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -2748,7 +2597,7 @@
         <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2766,32 +2615,18 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="L14" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="M14" t="s">
-        <v>310</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>0</v>
-      </c>
-      <c r="R14" s="1">
-        <v>0</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>309</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -2807,7 +2642,7 @@
         <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -2825,32 +2660,18 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="L15" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="M15" t="s">
-        <v>310</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>0</v>
-      </c>
-      <c r="R15" s="1">
-        <v>0</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>309</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -2866,7 +2687,7 @@
         <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -2884,32 +2705,18 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
+        <v>330</v>
+      </c>
+      <c r="L16" t="s">
         <v>334</v>
       </c>
-      <c r="L16" t="s">
-        <v>340</v>
-      </c>
       <c r="M16" t="s">
-        <v>310</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>0</v>
-      </c>
-      <c r="R16" s="1">
-        <v>0</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>309</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -2925,7 +2732,7 @@
         <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -2933,65 +2740,39 @@
       <c r="G17">
         <v>0</v>
       </c>
-      <c r="H17" t="s">
-        <v>338</v>
-      </c>
-      <c r="I17" t="s">
-        <v>338</v>
-      </c>
       <c r="J17" t="s">
-        <v>353</v>
-      </c>
-      <c r="K17" t="s">
-        <v>338</v>
-      </c>
-      <c r="L17" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="M17" t="s">
-        <v>308</v>
-      </c>
-      <c r="N17" t="s">
-        <v>338</v>
-      </c>
-      <c r="O17" t="s">
-        <v>338</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="17" t="s">
         <v>62</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>299</v>
+        <v>350</v>
       </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -3004,15 +2785,13 @@
       <c r="D19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>302</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
@@ -3025,9 +2804,7 @@
       <c r="D20" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>302</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
@@ -3047,7 +2824,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -3055,44 +2832,15 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
-        <v>338</v>
-      </c>
-      <c r="I21" t="s">
-        <v>338</v>
-      </c>
       <c r="J21" t="s">
-        <v>315</v>
-      </c>
-      <c r="K21" t="s">
-        <v>338</v>
-      </c>
-      <c r="L21" t="s">
-        <v>338</v>
-      </c>
-      <c r="M21" t="s">
-        <v>338</v>
-      </c>
-      <c r="N21" t="s">
-        <v>338</v>
-      </c>
-      <c r="O21" t="s">
-        <v>338</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
@@ -3106,14 +2854,14 @@
         <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>298</v>
+        <v>349</v>
       </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -3127,14 +2875,14 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>298</v>
+        <v>349</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
@@ -3148,7 +2896,7 @@
         <v>81</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -3166,28 +2914,14 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>309</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>0</v>
-      </c>
-      <c r="R24" s="1">
-        <v>0</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -3201,14 +2935,14 @@
         <v>85</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>298</v>
+        <v>349</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
@@ -3222,14 +2956,14 @@
         <v>89</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>298</v>
+        <v>349</v>
       </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
@@ -3243,14 +2977,14 @@
         <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>298</v>
+        <v>350</v>
       </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -3264,14 +2998,14 @@
         <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>298</v>
+        <v>350</v>
       </c>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -3285,7 +3019,7 @@
         <v>113</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3303,28 +3037,14 @@
         <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>309</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-      <c r="P29" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>0</v>
-      </c>
-      <c r="R29" s="1">
-        <v>0</v>
-      </c>
-      <c r="S29" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
@@ -3337,15 +3057,13 @@
       <c r="D30" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>302</v>
-      </c>
+      <c r="E30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>118</v>
       </c>
@@ -3358,15 +3076,13 @@
       <c r="D31" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>302</v>
-      </c>
+      <c r="E31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3397,10 +3113,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3408,15 +3124,15 @@
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="5" width="28.44140625" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.21875" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" customWidth="1"/>
-    <col min="16" max="16" width="11.77734375" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" customWidth="1"/>
-    <col min="18" max="18" width="20.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="15" max="15" width="11.77734375" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>122</v>
       </c>
@@ -3430,49 +3146,46 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>313</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="K1" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="I1" s="18" t="s">
-        <v>305</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>307</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>339</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>328</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="P1" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>331</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L1" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3486,7 +3199,7 @@
         <v>125</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3497,38 +3210,21 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K2" t="s">
-        <v>308</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I2" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J2" t="s">
+        <v>305</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -3542,7 +3238,7 @@
         <v>128</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -3553,38 +3249,21 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K3" t="s">
-        <v>308</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I3" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J3" t="s">
+        <v>305</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3598,7 +3277,7 @@
         <v>131</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -3609,38 +3288,21 @@
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K4" t="s">
-        <v>308</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I4" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J4" t="s">
+        <v>305</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -3654,7 +3316,7 @@
         <v>134</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3665,38 +3327,21 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K5" t="s">
-        <v>308</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I5" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J5" t="s">
+        <v>305</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -3710,7 +3355,7 @@
         <v>137</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -3721,38 +3366,21 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K6" t="s">
-        <v>308</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I6" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J6" t="s">
+        <v>305</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -3766,7 +3394,7 @@
         <v>212</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3777,38 +3405,21 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K7" t="s">
-        <v>308</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I7" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J7" t="s">
+        <v>305</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -3822,47 +3433,34 @@
         <v>141</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>338</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
       </c>
-      <c r="J8" s="1">
-        <v>0</v>
+      <c r="J8" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="K8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="1">
         <v>1</v>
       </c>
-      <c r="M8" s="1">
-        <v>1</v>
-      </c>
-      <c r="N8" s="1">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1">
-        <v>0</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -3876,47 +3474,44 @@
         <v>144</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>340</v>
+        <v>305</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
       </c>
       <c r="K9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="1">
         <v>1</v>
       </c>
       <c r="M9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="1">
         <v>0</v>
       </c>
-      <c r="O9" s="1">
-        <v>0</v>
+      <c r="O9" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>145</v>
       </c>
@@ -3930,7 +3525,7 @@
         <v>148</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>299</v>
+        <v>350</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -3944,9 +3539,8 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>149</v>
       </c>
@@ -3960,7 +3554,7 @@
         <v>151</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>299</v>
+        <v>350</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -3974,9 +3568,8 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>152</v>
       </c>
@@ -3990,7 +3583,7 @@
         <v>155</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -4001,38 +3594,31 @@
       <c r="H12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="K12" t="s">
-        <v>309</v>
-      </c>
-      <c r="L12" s="1">
-        <v>0</v>
-      </c>
+      <c r="I12" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="J12" t="s">
+        <v>306</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
       <c r="M12" s="1">
         <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
-      <c r="O12" s="1">
-        <v>0</v>
+      <c r="O12" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>63</v>
       </c>
@@ -4046,7 +3632,7 @@
         <v>158</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -4057,38 +3643,31 @@
       <c r="H13" s="1">
         <v>0</v>
       </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K13" t="s">
-        <v>309</v>
-      </c>
-      <c r="L13" s="1">
-        <v>0</v>
-      </c>
+      <c r="I13" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J13" t="s">
+        <v>306</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
       <c r="M13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="1">
-        <v>1</v>
-      </c>
-      <c r="O13" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>159</v>
       </c>
@@ -4102,7 +3681,7 @@
         <v>162</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -4113,38 +3692,31 @@
       <c r="H14" s="1">
         <v>0</v>
       </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="K14" t="s">
-        <v>309</v>
-      </c>
-      <c r="L14" s="1">
-        <v>0</v>
-      </c>
+      <c r="I14" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="J14" t="s">
+        <v>306</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
       <c r="M14" s="1">
         <v>0</v>
       </c>
       <c r="N14" s="1">
         <v>0</v>
       </c>
-      <c r="O14" s="1">
-        <v>0</v>
+      <c r="O14" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>163</v>
       </c>
@@ -4158,7 +3730,7 @@
         <v>166</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -4169,38 +3741,31 @@
       <c r="H15" s="1">
         <v>0</v>
       </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K15" t="s">
-        <v>309</v>
-      </c>
-      <c r="L15" s="1">
-        <v>0</v>
-      </c>
+      <c r="I15" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J15" t="s">
+        <v>306</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
       <c r="M15" s="1">
         <v>0</v>
       </c>
       <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>167</v>
       </c>
@@ -4214,49 +3779,32 @@
         <v>170</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="1">
         <v>0</v>
       </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="L16" s="1">
-        <v>0</v>
-      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
       <c r="M16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="1">
         <v>1</v>
       </c>
-      <c r="O16" s="1">
-        <v>1</v>
+      <c r="O16" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>171</v>
       </c>
@@ -4270,7 +3818,7 @@
         <v>170</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -4284,9 +3832,8 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>174</v>
       </c>
@@ -4300,49 +3847,32 @@
         <v>213</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="L18" s="1">
-        <v>0</v>
-      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
       <c r="M18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="1">
         <v>1</v>
       </c>
-      <c r="O18" s="1">
-        <v>1</v>
+      <c r="O18" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>177</v>
       </c>
@@ -4356,7 +3886,7 @@
         <v>213</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -4370,9 +3900,8 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
@@ -4386,7 +3915,7 @@
         <v>182</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -4397,38 +3926,21 @@
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K20" t="s">
-        <v>308</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20" s="1">
-        <v>0</v>
-      </c>
-      <c r="O20" s="1">
-        <v>0</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I20" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J20" t="s">
+        <v>305</v>
+      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
       <c r="Q20" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
@@ -4442,7 +3954,7 @@
         <v>182</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -4456,9 +3968,8 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>185</v>
       </c>
@@ -4472,7 +3983,7 @@
         <v>188</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -4483,38 +3994,21 @@
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K22" t="s">
-        <v>308</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22" s="1">
-        <v>0</v>
-      </c>
-      <c r="O22" s="1">
-        <v>0</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I22" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J22" t="s">
+        <v>305</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
       <c r="Q22" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -4528,7 +4022,7 @@
         <v>188</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -4542,9 +4036,8 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -4558,7 +4051,7 @@
         <v>193</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -4569,38 +4062,21 @@
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K24" t="s">
-        <v>308</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1">
-        <v>0</v>
-      </c>
-      <c r="O24" s="1">
-        <v>0</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I24" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J24" t="s">
+        <v>305</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
       <c r="Q24" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>86</v>
       </c>
@@ -4614,7 +4090,7 @@
         <v>196</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -4625,38 +4101,21 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K25" t="s">
-        <v>308</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25" s="1">
-        <v>0</v>
-      </c>
-      <c r="O25" s="1">
-        <v>0</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I25" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J25" t="s">
+        <v>305</v>
+      </c>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
       <c r="Q25" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>197</v>
       </c>
@@ -4670,7 +4129,7 @@
         <v>200</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -4681,38 +4140,21 @@
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K26" t="s">
-        <v>308</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26" s="1">
-        <v>0</v>
-      </c>
-      <c r="O26" s="1">
-        <v>0</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I26" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J26" t="s">
+        <v>305</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
       <c r="Q26" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>201</v>
       </c>
@@ -4726,7 +4168,7 @@
         <v>204</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -4737,38 +4179,21 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K27" t="s">
-        <v>308</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27" s="1">
-        <v>0</v>
-      </c>
-      <c r="O27" s="1">
-        <v>0</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I27" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J27" t="s">
+        <v>305</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
       <c r="Q27" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>205</v>
       </c>
@@ -4782,7 +4207,7 @@
         <v>208</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -4793,38 +4218,21 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K28" t="s">
-        <v>308</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1">
-        <v>0</v>
-      </c>
-      <c r="O28" s="1">
-        <v>0</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="I28" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J28" t="s">
+        <v>305</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -4838,7 +4246,7 @@
         <v>208</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -4852,7 +4260,6 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5044,145 +4451,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14">
-        <v>0</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="A2" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="B3" s="15">
-        <v>1</v>
-      </c>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="14" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="14" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="14">
         <v>28</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="14" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="13">
         <v>29</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="13" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="14">
         <v>30</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="14" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="13">
         <v>31</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="13" t="s">
         <v>296</v>
       </c>
     </row>
@@ -5254,7 +4661,7 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>255</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5276,10 +4683,10 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>245</v>
       </c>
     </row>
@@ -5287,10 +4694,10 @@
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Phase 1 Part 3: Load Instruction Variations are implemented and tested | PC block is fixed
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D041EF-96D8-4BC5-856F-53C4762348FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A15BB5-8F2A-4797-90D7-AD1AC197BC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main ISA" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="352">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -1112,10 +1112,13 @@
     <t>Phase 1 - Assignement 3 [1]</t>
   </si>
   <si>
-    <t>Phase 1 - Assignement 3 [2]</t>
-  </si>
-  <si>
     <t>Phase 2</t>
+  </si>
+  <si>
+    <t>wb_se_select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DONE] Phase 1 - Assignement 3 </t>
   </si>
 </sst>
 </file>
@@ -1276,7 +1279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1325,12 +1328,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1723,9 +1720,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:S32" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
-  <autoFilter ref="A1:S32" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:T32" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A1:T32" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}"/>
+  <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="46"/>
     <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="45"/>
     <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="44"/>
@@ -1738,6 +1735,7 @@
     <tableColumn id="10" xr3:uid="{0153894A-151B-41AD-B603-B7BF55EEBE9C}" name="Write_back_sel" dataDxfId="37"/>
     <tableColumn id="11" xr3:uid="{C68ADF0D-C375-4115-93EF-CD4021B0BD3E}" name="AluOp" dataDxfId="36"/>
     <tableColumn id="20" xr3:uid="{4B7A4639-28F0-4297-B746-1FB610AB5BC3}" name="AluOp_immediate"/>
+    <tableColumn id="18" xr3:uid="{8FFAE8F4-2929-40DB-8CDB-B6B62F5A5B1D}" name="wb_se_select"/>
     <tableColumn id="21" xr3:uid="{83AF33B5-363D-492B-8E5C-C63E2DB98A90}" name="se_select"/>
     <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="35"/>
     <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="PC Src" dataDxfId="34"/>
@@ -2064,10 +2062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView zoomScale="127" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2078,11 +2076,11 @@
     <col min="4" max="4" width="32.5546875" customWidth="1"/>
     <col min="5" max="5" width="36.5546875" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="12" max="12" width="14.21875" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.21875" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2120,28 +2118,31 @@
         <v>344</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="R1" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2155,12 +2156,12 @@
         <v>7</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
@@ -2194,18 +2195,18 @@
       <c r="K3" t="s">
         <v>307</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
         <v>339</v>
       </c>
-      <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2221,18 +2222,18 @@
       <c r="E4" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
       <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2266,18 +2267,18 @@
       <c r="K5" t="s">
         <v>306</v>
       </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
       <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2308,18 +2309,18 @@
       <c r="K6" t="s">
         <v>307</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
         <v>347</v>
       </c>
-      <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2353,18 +2354,18 @@
       <c r="K7" t="s">
         <v>307</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
         <v>338</v>
       </c>
-      <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -2398,18 +2399,18 @@
       <c r="K8" t="s">
         <v>307</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
         <v>340</v>
       </c>
-      <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -2443,18 +2444,18 @@
       <c r="K9" t="s">
         <v>307</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
         <v>341</v>
       </c>
-      <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2488,36 +2489,36 @@
       <c r="L10" t="s">
         <v>312</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>306</v>
       </c>
-      <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -2554,15 +2555,15 @@
       <c r="L12" t="s">
         <v>313</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>306</v>
       </c>
-      <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -2578,12 +2579,12 @@
       <c r="E13" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2620,15 +2621,15 @@
       <c r="L14" t="s">
         <v>310</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>307</v>
       </c>
-      <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -2665,15 +2666,15 @@
       <c r="L15" t="s">
         <v>345</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>307</v>
       </c>
-      <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2710,15 +2711,15 @@
       <c r="L16" t="s">
         <v>334</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>307</v>
       </c>
-      <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -2743,36 +2744,36 @@
       <c r="J17" t="s">
         <v>346</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>305</v>
       </c>
-      <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-    </row>
-    <row r="18" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="P18" s="1"/>
+        <v>349</v>
+      </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -2786,12 +2787,12 @@
         <v>66</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-    </row>
-    <row r="20" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
@@ -2805,12 +2806,12 @@
         <v>101</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-    </row>
-    <row r="21" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="T20" s="1"/>
+    </row>
+    <row r="21" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -2835,12 +2836,12 @@
       <c r="J21" t="s">
         <v>311</v>
       </c>
-      <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
@@ -2854,14 +2855,35 @@
         <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="P22" s="1"/>
+        <v>351</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>314</v>
+      </c>
+      <c r="K22" t="s">
+        <v>306</v>
+      </c>
+      <c r="M22" t="s">
+        <v>345</v>
+      </c>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T22" s="1"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -2875,14 +2897,35 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="P23" s="1"/>
+        <v>351</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>314</v>
+      </c>
+      <c r="K23" t="s">
+        <v>306</v>
+      </c>
+      <c r="M23" t="s">
+        <v>312</v>
+      </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T23" s="1"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
@@ -2896,7 +2939,7 @@
         <v>81</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>342</v>
+        <v>299</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -2916,12 +2959,12 @@
       <c r="K24" t="s">
         <v>306</v>
       </c>
-      <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T24" s="1"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -2935,14 +2978,35 @@
         <v>85</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="P25" s="1"/>
+        <v>351</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>314</v>
+      </c>
+      <c r="K25" t="s">
+        <v>306</v>
+      </c>
+      <c r="M25" t="s">
+        <v>334</v>
+      </c>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T25" s="1"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
@@ -2956,14 +3020,35 @@
         <v>89</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="P26" s="1"/>
+        <v>351</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>314</v>
+      </c>
+      <c r="K26" t="s">
+        <v>306</v>
+      </c>
+      <c r="M26" t="s">
+        <v>313</v>
+      </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T26" s="1"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
@@ -2977,14 +3062,14 @@
         <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="P27" s="1"/>
+        <v>349</v>
+      </c>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -2998,14 +3083,14 @@
         <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="P28" s="1"/>
+        <v>349</v>
+      </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T28" s="1"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -3039,12 +3124,12 @@
       <c r="K29" t="s">
         <v>306</v>
       </c>
-      <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T29" s="1"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
@@ -3058,12 +3143,12 @@
         <v>117</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T30" s="1"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>118</v>
       </c>
@@ -3077,12 +3162,12 @@
         <v>121</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T31" s="1"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3094,12 +3179,12 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3115,8 +3200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="E2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3512,20 +3597,20 @@
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -3541,20 +3626,20 @@
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>

</xml_diff>

<commit_message>
Phase 1 Part 3: Unsigned Instructions is completed and Tested
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A15BB5-8F2A-4797-90D7-AD1AC197BC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A36D99-F4FA-4B4B-921A-914B2E9B8751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main ISA" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="354">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -977,9 +977,6 @@
     <t>AluOp</t>
   </si>
   <si>
-    <t>Jump</t>
-  </si>
-  <si>
     <t>2'b10</t>
   </si>
   <si>
@@ -1109,9 +1106,6 @@
     <t>e_zero</t>
   </si>
   <si>
-    <t>Phase 1 - Assignement 3 [1]</t>
-  </si>
-  <si>
     <t>Phase 2</t>
   </si>
   <si>
@@ -1119,6 +1113,18 @@
   </si>
   <si>
     <t xml:space="preserve">[DONE] Phase 1 - Assignement 3 </t>
+  </si>
+  <si>
+    <t>Overflow Mask</t>
+  </si>
+  <si>
+    <t>overflow Mask</t>
+  </si>
+  <si>
+    <t>1'b1</t>
+  </si>
+  <si>
+    <t>1'b0</t>
   </si>
 </sst>
 </file>
@@ -1737,7 +1743,7 @@
     <tableColumn id="20" xr3:uid="{4B7A4639-28F0-4297-B746-1FB610AB5BC3}" name="AluOp_immediate"/>
     <tableColumn id="18" xr3:uid="{8FFAE8F4-2929-40DB-8CDB-B6B62F5A5B1D}" name="wb_se_select"/>
     <tableColumn id="21" xr3:uid="{83AF33B5-363D-492B-8E5C-C63E2DB98A90}" name="se_select"/>
-    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Jump" dataDxfId="35"/>
+    <tableColumn id="12" xr3:uid="{F1D4D373-D3C9-4BF4-9941-4766A9F778CF}" name="Overflow Mask" dataDxfId="35"/>
     <tableColumn id="13" xr3:uid="{E4CE9616-85BB-465A-8E96-A5EC285FC9E7}" name="PC Src" dataDxfId="34"/>
     <tableColumn id="14" xr3:uid="{65386F80-7AF9-4CF2-BDE0-29D2094B577A}" name="hi_write" dataDxfId="33"/>
     <tableColumn id="15" xr3:uid="{FA558C62-1F5B-4CE1-A1DE-149585FE9142}" name="lo_write" dataDxfId="32"/>
@@ -1762,7 +1768,7 @@
     <tableColumn id="14" xr3:uid="{B2AB814A-4427-483D-92F7-16C5C8659619}" name="AluSrc" dataDxfId="20"/>
     <tableColumn id="16" xr3:uid="{D1503AC1-DA6F-431E-86E3-3CD8BAD27F47}" name="Write_Back_sel" dataDxfId="19"/>
     <tableColumn id="17" xr3:uid="{03DAA7C4-6940-4324-93F3-3F703363AC9E}" name="AluOp" dataDxfId="18"/>
-    <tableColumn id="18" xr3:uid="{B4769B34-7E40-48A1-81CF-AF31CD8F17DF}" name="Jump" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{B4769B34-7E40-48A1-81CF-AF31CD8F17DF}" name="overflow Mask" dataDxfId="17"/>
     <tableColumn id="19" xr3:uid="{804568FB-85BF-40E3-B057-9BD0161489CA}" name="PCsrc" dataDxfId="16"/>
     <tableColumn id="8" xr3:uid="{E7BF6538-000F-4221-BEAF-1B1069F544DF}" name="hi_write" dataDxfId="15"/>
     <tableColumn id="9" xr3:uid="{EB15F963-101B-4FD6-8C35-479C603DBCE6}" name="lo_write" dataDxfId="14"/>
@@ -2064,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="L4" zoomScale="176" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O13" sqref="O12:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2077,6 +2083,7 @@
     <col min="5" max="5" width="36.5546875" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="12" max="13" width="14.21875" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2097,7 +2104,7 @@
         <v>298</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>300</v>
@@ -2109,37 +2116,37 @@
         <v>302</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>303</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>304</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q1" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="R1" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>326</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -2175,7 +2182,7 @@
         <v>93</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2193,13 +2200,10 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>307</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
+        <v>306</v>
       </c>
       <c r="P3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -2222,11 +2226,8 @@
       <c r="E4" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
+      <c r="P4" t="s">
+        <v>304</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -2247,31 +2248,28 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
+        <v>304</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>333</v>
+      </c>
+      <c r="K5" t="s">
         <v>305</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>334</v>
-      </c>
-      <c r="K5" t="s">
-        <v>306</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
+      <c r="P5" t="s">
+        <v>304</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -2292,7 +2290,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2307,13 +2305,10 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>307</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
+        <v>306</v>
       </c>
       <c r="P6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -2334,7 +2329,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2352,13 +2347,10 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>307</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
+        <v>306</v>
       </c>
       <c r="P7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -2379,7 +2371,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -2397,13 +2389,10 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>307</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
+        <v>306</v>
       </c>
       <c r="P8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -2424,7 +2413,7 @@
         <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2442,13 +2431,10 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>307</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
+        <v>306</v>
       </c>
       <c r="P9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -2484,13 +2470,16 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N10" t="s">
-        <v>306</v>
+        <v>305</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -2511,7 +2500,10 @@
         <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -2532,7 +2524,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -2550,13 +2542,13 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -2577,7 +2569,7 @@
         <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -2598,7 +2590,7 @@
         <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2616,13 +2608,13 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -2643,7 +2635,7 @@
         <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -2661,13 +2653,13 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="N15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2688,7 +2680,7 @@
         <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -2706,13 +2698,13 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -2733,7 +2725,7 @@
         <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -2742,10 +2734,10 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="N17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -2766,7 +2758,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -2825,7 +2817,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2834,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
@@ -2855,7 +2847,7 @@
         <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -2870,13 +2862,13 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -2897,7 +2889,7 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -2912,13 +2904,13 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
@@ -2957,7 +2949,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -2978,7 +2970,7 @@
         <v>85</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -2993,13 +2985,13 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M25" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -3020,7 +3012,7 @@
         <v>89</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -3035,13 +3027,13 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -3062,7 +3054,7 @@
         <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
@@ -3083,7 +3075,7 @@
         <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -3104,7 +3096,7 @@
         <v>113</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3122,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
@@ -3200,8 +3192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3210,6 +3202,7 @@
     <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="5" width="28.44140625" customWidth="1"/>
     <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.21875" customWidth="1"/>
     <col min="14" max="14" width="12.6640625" customWidth="1"/>
     <col min="15" max="15" width="11.77734375" customWidth="1"/>
@@ -3234,7 +3227,7 @@
         <v>298</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>300</v>
@@ -3243,31 +3236,31 @@
         <v>301</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>303</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>304</v>
+        <v>351</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M1" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="P1" s="16" t="s">
-        <v>327</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -3284,7 +3277,7 @@
         <v>125</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3296,17 +3289,17 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -3323,7 +3316,7 @@
         <v>128</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -3335,17 +3328,17 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -3362,7 +3355,7 @@
         <v>131</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -3374,17 +3367,17 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -3401,7 +3394,7 @@
         <v>134</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3413,17 +3406,17 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -3440,7 +3433,7 @@
         <v>137</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -3452,17 +3445,17 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -3479,7 +3472,7 @@
         <v>212</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3491,17 +3484,17 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -3518,32 +3511,32 @@
         <v>141</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1</v>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="1" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -3559,28 +3552,26 @@
         <v>144</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
       </c>
-      <c r="K9" s="1">
-        <v>1</v>
-      </c>
-      <c r="L9" s="1">
-        <v>1</v>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
@@ -3589,12 +3580,14 @@
         <v>0</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q9" s="1"/>
+        <v>328</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -3610,7 +3603,7 @@
         <v>148</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -3639,7 +3632,7 @@
         <v>151</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -3668,7 +3661,7 @@
         <v>155</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -3680,10 +3673,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="J12" t="s">
         <v>305</v>
-      </c>
-      <c r="J12" t="s">
-        <v>306</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -3694,13 +3687,13 @@
         <v>0</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -3717,7 +3710,7 @@
         <v>158</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -3729,10 +3722,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -3743,13 +3736,13 @@
         <v>0</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="Q13" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -3766,7 +3759,7 @@
         <v>162</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -3778,10 +3771,10 @@
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -3792,13 +3785,13 @@
         <v>0</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -3815,7 +3808,7 @@
         <v>166</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -3827,10 +3820,10 @@
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -3841,13 +3834,13 @@
         <v>1</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -3864,7 +3857,7 @@
         <v>170</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1">
@@ -3882,10 +3875,10 @@
         <v>1</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q16" s="1"/>
     </row>
@@ -3902,9 +3895,7 @@
       <c r="D17" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>348</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -3932,7 +3923,7 @@
         <v>213</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1">
@@ -3950,10 +3941,10 @@
         <v>1</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Q18" s="1"/>
     </row>
@@ -3970,9 +3961,7 @@
       <c r="D19" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>348</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -4012,17 +4001,20 @@
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J20" t="s">
-        <v>305</v>
+        <v>304</v>
+      </c>
+      <c r="K20" t="s">
+        <v>352</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -4039,14 +4031,16 @@
         <v>182</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -4080,17 +4074,20 @@
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J22" t="s">
-        <v>305</v>
+        <v>304</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -4107,14 +4104,16 @@
         <v>188</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+      <c r="K23" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -4148,17 +4147,18 @@
         <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J24" t="s">
-        <v>305</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="K24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -4187,17 +4187,18 @@
         <v>0</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J25" t="s">
-        <v>305</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="K25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
@@ -4214,7 +4215,7 @@
         <v>200</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -4226,17 +4227,18 @@
         <v>0</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J26" t="s">
-        <v>305</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="K26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -4253,7 +4255,7 @@
         <v>204</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -4265,17 +4267,18 @@
         <v>0</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J27" t="s">
-        <v>305</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="K27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -4304,17 +4307,18 @@
         <v>0</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J28" t="s">
-        <v>305</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="K28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -4331,7 +4335,7 @@
         <v>208</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>

</xml_diff>

<commit_message>
Phase 1 Part 3: Passing the Direct Tests
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A36D99-F4FA-4B4B-921A-914B2E9B8751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C191B85C-15E4-4744-89FF-D1831BB81B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main ISA" sheetId="1" r:id="rId1"/>
@@ -2070,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView topLeftCell="L4" zoomScale="176" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="176" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="O13" sqref="O12:O13"/>
     </sheetView>
   </sheetViews>
@@ -3192,8 +3192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4528,8 +4528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF87FDE8-CD08-404C-B3EB-3F68C8774AD2}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Phase 1 Part3: Mips Core is Synthesised successfully except the divider block
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C191B85C-15E4-4744-89FF-D1831BB81B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB33A59-31E7-4E8F-8024-91C0063182F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main ISA" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="355">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -1125,6 +1125,9 @@
   </si>
   <si>
     <t>1'b0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DONE] Phase 1 - Assignement 2 [Not Synthesised] </t>
   </si>
 </sst>
 </file>
@@ -2070,7 +2073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView zoomScale="176" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="176" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="O13" sqref="O12:O13"/>
     </sheetView>
   </sheetViews>
@@ -3192,8 +3195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3923,7 +3926,7 @@
         <v>213</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1">
@@ -4528,7 +4531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF87FDE8-CD08-404C-B3EB-3F68C8774AD2}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="112" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Phase 1 is Complete
</commit_message>
<xml_diff>
--- a/docs/MIPS I ISA.xlsx
+++ b/docs/MIPS I ISA.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital\SoC\mips_top\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB33A59-31E7-4E8F-8024-91C0063182F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2371D3D4-A0C2-4C68-8323-3F3C1DAB6AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main ISA" sheetId="1" r:id="rId1"/>
     <sheet name="R-Type" sheetId="2" r:id="rId2"/>
-    <sheet name="F-Type" sheetId="3" r:id="rId3"/>
-    <sheet name="Register File" sheetId="5" r:id="rId4"/>
-    <sheet name="Verification Plan" sheetId="4" r:id="rId5"/>
+    <sheet name="Controls" sheetId="6" r:id="rId3"/>
+    <sheet name="F-Type" sheetId="3" r:id="rId4"/>
+    <sheet name="Register File" sheetId="5" r:id="rId5"/>
+    <sheet name="Verification Plan" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="434">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -1128,6 +1129,243 @@
   </si>
   <si>
     <t xml:space="preserve">[DONE] Phase 1 - Assignement 2 [Not Synthesised] </t>
+  </si>
+  <si>
+    <t>PC = PC Plus 4</t>
+  </si>
+  <si>
+    <t>PC = BTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC = JTA </t>
+  </si>
+  <si>
+    <t>PC = RegFile Data</t>
+  </si>
+  <si>
+    <t>[3 bits] Control Type of Extention of Immediate</t>
+  </si>
+  <si>
+    <t>[3 bits] Control Next PC</t>
+  </si>
+  <si>
+    <t>SignImm =  SignExtented  Immediate</t>
+  </si>
+  <si>
+    <t>SignImm =  ZeroExtented  Immediate</t>
+  </si>
+  <si>
+    <t>SignImm = Load Upper Immediate</t>
+  </si>
+  <si>
+    <t>Not used</t>
+  </si>
+  <si>
+    <t>[3 bit] Chose the Write back Data</t>
+  </si>
+  <si>
+    <t>[3 bit] Control Type of Extention in Mem read data</t>
+  </si>
+  <si>
+    <t>mem_se_data =  SignExtented{readdata[15:0]}</t>
+  </si>
+  <si>
+    <t>mem_se_data =  ZeroExtented{readdata[15:0]}</t>
+  </si>
+  <si>
+    <t>mem_se_data =  SignExtented{readdata[7:0]}</t>
+  </si>
+  <si>
+    <t>mem_se_data =  ZeroExtented{readdata[7:0]}</t>
+  </si>
+  <si>
+    <t>[2 bit] Control Operand B data Source</t>
+  </si>
+  <si>
+    <t>operand_b = data_rt</t>
+  </si>
+  <si>
+    <t>operand_b = SignImm</t>
+  </si>
+  <si>
+    <t>operand_b = 0</t>
+  </si>
+  <si>
+    <t>[2 bit] Control Register File Write Back Address</t>
+  </si>
+  <si>
+    <t>wb_addr = instr_rt</t>
+  </si>
+  <si>
+    <t>wb_addr = 31 "$ra"</t>
+  </si>
+  <si>
+    <t>wb_addr = instr_rd</t>
+  </si>
+  <si>
+    <t>[1 bit] Write Enable of Register File</t>
+  </si>
+  <si>
+    <t>RegWrite</t>
+  </si>
+  <si>
+    <t>No Write back in RegFile</t>
+  </si>
+  <si>
+    <t>Write back in RegFile</t>
+  </si>
+  <si>
+    <t>[4 bits] Control The operation in ALU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alu_result = op_a &amp; op_b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">alu_result = op_a | op_b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">alu_result = op_a + op_b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">alu_result = op_a ^ op_b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">alu_result = ~(op_a | op_b) </t>
+  </si>
+  <si>
+    <t>alu_result = (op_a &lt; op_b) "Unsigned"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alu_result = op_a - op_b </t>
+  </si>
+  <si>
+    <t>alu_result = (op_a &lt; op_b) "Signed"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alu_result = op_b &lt;&lt; shmat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">alu_result = op_b &gt;&gt; shmat </t>
+  </si>
+  <si>
+    <t>alu_result = op_b &gt;&gt;&gt; shmat "Signed"</t>
+  </si>
+  <si>
+    <t>Not Used</t>
+  </si>
+  <si>
+    <t>alu_result = op_b &gt;&gt;&gt; op_a[4:0] "Signed"</t>
+  </si>
+  <si>
+    <t>alu_result = op_b &gt;&gt; op_a[4:0]</t>
+  </si>
+  <si>
+    <t>alu_result = op_b &lt;&lt; op_a[4:0]</t>
+  </si>
+  <si>
+    <t>wb_data = aluout</t>
+  </si>
+  <si>
+    <t>wb_data = readdata</t>
+  </si>
+  <si>
+    <t>wb_data = hi_reg</t>
+  </si>
+  <si>
+    <t>wb_data = lo_reg</t>
+  </si>
+  <si>
+    <t>wb_data = pc_plus4</t>
+  </si>
+  <si>
+    <t>wb_data = signImm</t>
+  </si>
+  <si>
+    <t>wb_data = mult_lo</t>
+  </si>
+  <si>
+    <t>wb_data = mem_se_data</t>
+  </si>
+  <si>
+    <t>Don't load in Hi reg</t>
+  </si>
+  <si>
+    <t>Load in Hi reg</t>
+  </si>
+  <si>
+    <t>[1 bit] loading in lo reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1 bit] loading in hi reg </t>
+  </si>
+  <si>
+    <t>Don't load in Lo register</t>
+  </si>
+  <si>
+    <t>Load in Lo register</t>
+  </si>
+  <si>
+    <t>[2 bits] hi register data source selection</t>
+  </si>
+  <si>
+    <t>[2 bits] lo register data source selection</t>
+  </si>
+  <si>
+    <t>hi_reg = hi_reg</t>
+  </si>
+  <si>
+    <t>hi_reg = reg_file</t>
+  </si>
+  <si>
+    <t>hi_reg = mult_hi</t>
+  </si>
+  <si>
+    <t>hi_reg = div_hi</t>
+  </si>
+  <si>
+    <t>lo_reg = lo_reg</t>
+  </si>
+  <si>
+    <t>lo_reg = reg_file</t>
+  </si>
+  <si>
+    <t>lo_reg = mult_lo</t>
+  </si>
+  <si>
+    <t>lo_reg = div_lo</t>
+  </si>
+  <si>
+    <t>unsigned_mult</t>
+  </si>
+  <si>
+    <t>[1 bit] applying the overflow in the execption</t>
+  </si>
+  <si>
+    <t>There is an overflow output</t>
+  </si>
+  <si>
+    <t>There is NO overflow output</t>
+  </si>
+  <si>
+    <t>[1 bit] Determine the multiplication type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signed Multiplication </t>
+  </si>
+  <si>
+    <t>Unsigned Multiplication</t>
+  </si>
+  <si>
+    <t>unsigned_div</t>
+  </si>
+  <si>
+    <t>[1 bit] Determine the division type</t>
+  </si>
+  <si>
+    <t>signed division</t>
+  </si>
+  <si>
+    <t>Unsigned division</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1375,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1168,8 +1406,16 @@
       <color rgb="FF000000"/>
       <name val="Aptos"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1204,6 +1450,12 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -1288,7 +1540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1336,6 +1588,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1730,7 +1994,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:T32" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
-  <autoFilter ref="A1:T32" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}"/>
+  <autoFilter ref="A1:T32" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="[DONE] Phase 1 - Assignement 1"/>
+        <filter val="[DONE] Phase 1 - Assignement 2"/>
+        <filter val="[DONE] Phase 1 - Assignement 3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="46"/>
     <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="45"/>
@@ -1759,7 +2031,16 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:Q29" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A1:Q29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}"/>
+  <autoFilter ref="A1:Q29" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="[DONE] Phase 1 - Assignement 1"/>
+        <filter val="[DONE] Phase 1 - Assignement 2"/>
+        <filter val="[DONE] Phase 1 - Assignement 2 [Not Synthesised]"/>
+        <filter val="[DONE] Phase 1 - Assignement 3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="26"/>
@@ -2073,8 +2354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="176" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O13" sqref="O12:O13"/>
+    <sheetView topLeftCell="D1" zoomScale="176" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2152,7 +2433,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2747,7 +3028,7 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>94</v>
       </c>
@@ -2768,7 +3049,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -2787,7 +3068,7 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
@@ -3043,7 +3324,7 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
@@ -3064,7 +3345,7 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -3124,7 +3405,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
@@ -3143,7 +3424,7 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>118</v>
       </c>
@@ -3162,7 +3443,7 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3195,8 +3476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3592,7 +3873,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>145</v>
       </c>
@@ -3621,7 +3902,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>149</v>
       </c>
@@ -3885,7 +4166,7 @@
       </c>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>171</v>
       </c>
@@ -3951,7 +4232,7 @@
       </c>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>177</v>
       </c>
@@ -4364,11 +4645,730 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC34BEC-07EC-4D50-AC0B-49504B180A90}">
+  <dimension ref="A1:B102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="DX14" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:ET1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>11</v>
+      </c>
+      <c r="B55" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>12</v>
+      </c>
+      <c r="B56" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>13</v>
+      </c>
+      <c r="B57" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>15</v>
+      </c>
+      <c r="B59" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>4</v>
+      </c>
+      <c r="B66" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>7</v>
+      </c>
+      <c r="B69" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>0</v>
+      </c>
+      <c r="B81" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>1</v>
+      </c>
+      <c r="B82" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>2</v>
+      </c>
+      <c r="B83" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="B86" s="18" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>0</v>
+      </c>
+      <c r="B87" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>1</v>
+      </c>
+      <c r="B88" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>2</v>
+      </c>
+      <c r="B89" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>3</v>
+      </c>
+      <c r="B90" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B92" s="17" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="B93" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="B94" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="B96" s="17" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>1</v>
+      </c>
+      <c r="B98" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="17" t="s">
+        <v>430</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="B101" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>1</v>
+      </c>
+      <c r="B102" t="s">
+        <v>433</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A529840E-1C1E-4789-B7C1-A5C3FA17C3B9}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:ET1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4527,7 +5527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF87FDE8-CD08-404C-B3EB-3F68C8774AD2}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -4690,7 +5690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A87B3F1-8E67-4593-84BE-C265B2E04654}">
   <dimension ref="A1:C11"/>
   <sheetViews>

</xml_diff>